<commit_message>
changes to the labels
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C82FFC-3518-43AD-855E-AD1985EDB642}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{8FD1DAFA-8045-4ABA-877C-C4F83DA862DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -124,15 +124,9 @@
     <t>FRUITINGVEG_0202</t>
   </si>
   <si>
-    <t>fruiting vegetable intake [g/d]</t>
-  </si>
-  <si>
     <t>ROOTVEG_0203</t>
   </si>
   <si>
-    <t>root and tuber vegetable intake [g/d]</t>
-  </si>
-  <si>
     <t>CABBAGE_0204</t>
   </si>
   <si>
@@ -142,63 +136,33 @@
     <t>MUSHROOMS_0205</t>
   </si>
   <si>
-    <t>mushroom intake [g/d]</t>
-  </si>
-  <si>
     <t>GRAINPODVEG_0206</t>
   </si>
   <si>
-    <t>intake of legumes with pod [g/d]</t>
-  </si>
-  <si>
     <t>ONION_GARLIC_0207</t>
   </si>
   <si>
-    <t>bulb vegetables (onions, garlic) intake [g/d]</t>
-  </si>
-  <si>
     <t>STALKVEG_0208</t>
   </si>
   <si>
-    <t>intake of stems/stalks eaten as vegetables [g/d]</t>
-  </si>
-  <si>
     <t>MIXEDVEG_0209</t>
   </si>
   <si>
-    <t>intake of mixed vegetable salad or mixed green salad [g/d]</t>
-  </si>
-  <si>
     <t>LEGUMES_TOT_03</t>
   </si>
   <si>
-    <t>Legumes intake [g/d]</t>
-  </si>
-  <si>
     <t>LEGUMES_0301</t>
   </si>
   <si>
-    <t>intake fresh seeds (without pod) from legumes (beans, peas etc.) [g/d]</t>
-  </si>
-  <si>
     <t>FRUITS_TOT_04</t>
   </si>
   <si>
-    <t>intake of any type of RPCs of fruit nature [g/d]</t>
-  </si>
-  <si>
     <t>FRUITS_0401</t>
   </si>
   <si>
-    <t>Intake of fruits used as a fruit (as part-nature) [g/d]</t>
-  </si>
-  <si>
     <t>NUTS_SEEDS_0402</t>
   </si>
   <si>
-    <t>Intake of tree nuts and seeds (as plant) and from nuts and similar seeds (as part-nature) [g/d]</t>
-  </si>
-  <si>
     <t>MIXEDFRUITS_0403</t>
   </si>
   <si>
@@ -208,9 +172,6 @@
     <t>OLIVES_0404</t>
   </si>
   <si>
-    <t>Intake of processed olives, table olives and similar and olives for oil production and similar [g/d]</t>
-  </si>
-  <si>
     <t>DAIRY_05</t>
   </si>
   <si>
@@ -230,9 +191,6 @@
   </si>
   <si>
     <t>YOGURT_0503</t>
-  </si>
-  <si>
-    <t>Intake of fermented milk [g/d]</t>
   </si>
   <si>
     <t>CURD_0504</t>
@@ -294,15 +252,9 @@
     <t>PASTA_RICE_0602</t>
   </si>
   <si>
-    <t>Intake of pastas and rice (or other cereal) –based dishes and pastas and rice (or other cereal) –based dishes (as part-nature) [g/d]</t>
-  </si>
-  <si>
     <t>BREAD_PROD_0603</t>
   </si>
   <si>
-    <t>Intake of bread (as part-nature), bread products (as part-nature), bread and similar [g/d]</t>
-  </si>
-  <si>
     <t>BREAD_060301</t>
   </si>
   <si>
@@ -318,9 +270,6 @@
     <t>BREAKF_CEREALS_0604</t>
   </si>
   <si>
-    <t>Intake of breakfast cereals and breakfast cereals, plain [g/d]</t>
-  </si>
-  <si>
     <t>SALT_BISCUIT_0605</t>
   </si>
   <si>
@@ -366,69 +315,36 @@
     <t>MUTTON_LAMB_070104</t>
   </si>
   <si>
-    <t>Intake of Lamb and Sheep (adult) fresh meat [g/d]</t>
-  </si>
-  <si>
     <t>HORSE_070105</t>
   </si>
   <si>
-    <t>Intake of Horse fresh meat [g/d]</t>
-  </si>
-  <si>
     <t>GOAT_070106</t>
   </si>
   <si>
-    <t>Intake of Goat fresh meat, meat food and meat products [g/d]</t>
-  </si>
-  <si>
     <t>POULTRY_0702</t>
   </si>
   <si>
-    <t>Intake of poultry fresh meat (muscle meat) and poultry meat food [g/d]</t>
-  </si>
-  <si>
     <t>OTHERPOULTRY_070200</t>
   </si>
   <si>
-    <t>Intake of other poultry fresh meat, meat products, meat preparations and other poultry meat food [g/d]</t>
-  </si>
-  <si>
     <t>CHICKEN_070201</t>
   </si>
   <si>
-    <t>Intake of chicken fresh meat, meat food and meat products [g/d]</t>
-  </si>
-  <si>
     <t>TURKEY_070202</t>
   </si>
   <si>
-    <t>Intake of turkey fresh meat, meat food, meat products and meat preparations [g/d]</t>
-  </si>
-  <si>
     <t>DUCK_070203</t>
   </si>
   <si>
-    <t>Intake of duck fresh meat, meat food, meat products, meat preparations [g/d]</t>
-  </si>
-  <si>
     <t>GOOSE_070204</t>
   </si>
   <si>
-    <t>Intake of goose fresh meat, meat food, meat products and  meat preparations [g/d]</t>
-  </si>
-  <si>
     <t>RABBIT_070205</t>
   </si>
   <si>
-    <t>Intake of rabbit fresh meat, meat food, meat products and meat preparations [g/d]</t>
-  </si>
-  <si>
     <t>GAME_0703</t>
   </si>
   <si>
-    <t>Intake of Game mammals fresh meat/fat tissue, meat food, meat products, meat preparations, Game birds fresh meat, meat food, meat products, meat preparations and other game birds fresh meat [g/d]</t>
-  </si>
-  <si>
     <t>PROCMEAT_0704</t>
   </si>
   <si>
@@ -444,9 +360,6 @@
     <t>FISH_SHELLFISH_08</t>
   </si>
   <si>
-    <t>Intake of fish, seafood, amphibians, reptiles and invertebrates, products of animal origin - fish, fish products and any other marine and freshwater food products [g/d]</t>
-  </si>
-  <si>
     <t>FISH_0801</t>
   </si>
   <si>
@@ -462,10 +375,6 @@
     <t>FISH_PROD_0803</t>
   </si>
   <si>
-    <t>Intake of fish and seafood processed
-Fish fingers, breaded [g/d]</t>
-  </si>
-  <si>
     <t>EGG_PROD_09</t>
   </si>
   <si>
@@ -475,21 +384,12 @@
     <t>EGGS_0901</t>
   </si>
   <si>
-    <t>Intake of liquid egg products, hardened egg products, boiled eggs products, fried eggs products and processed eggs and egg products [g/d]</t>
-  </si>
-  <si>
     <t>FAT_10</t>
   </si>
   <si>
-    <t>Intake of animal and vegetable fats and oils and primary derivatives thereof [g/d]</t>
-  </si>
-  <si>
     <t>VEGOILS_1001</t>
   </si>
   <si>
-    <t>Intake of vegetable fats and oils, edible [g/d]</t>
-  </si>
-  <si>
     <t>BUTTER_1002</t>
   </si>
   <si>
@@ -511,15 +411,9 @@
     <t>MARINEOILS_1005</t>
   </si>
   <si>
-    <t>Intake of fats and oils from marine animals [g/d]</t>
-  </si>
-  <si>
     <t>OTHER_ANIMALFAT_1006</t>
   </si>
   <si>
-    <t>Intake of animal fats and oils (processed fat from animal tissue) [g/d]</t>
-  </si>
-  <si>
     <t>SUGAR_CONFECT_11</t>
   </si>
   <si>
@@ -553,9 +447,6 @@
     <t>ICECREAM_1105</t>
   </si>
   <si>
-    <t>Intake of spoonable desserts and ice creams (generic) [g/d]</t>
-  </si>
-  <si>
     <t>ICECREAM_MILK_110501</t>
   </si>
   <si>
@@ -601,15 +492,9 @@
     <t>FRUITVEG_JUICE_1301</t>
   </si>
   <si>
-    <t>Intake of fruit and vegetable juices and nectars [g/d]</t>
-  </si>
-  <si>
     <t>SOFTDRINKS_1302</t>
   </si>
   <si>
-    <t>Intake of soft drinks (flavoured, no fruit) [g/d]</t>
-  </si>
-  <si>
     <t>HOTDRINKS_1303</t>
   </si>
   <si>
@@ -661,9 +546,6 @@
     <t>FORTWINE_1402</t>
   </si>
   <si>
-    <t>Intake of fortified/liqueur wine (as part-nature) [g/d]</t>
-  </si>
-  <si>
     <t>BEER_1403</t>
   </si>
   <si>
@@ -715,15 +597,9 @@
     <t>DRESSINGS_150102</t>
   </si>
   <si>
-    <t>Salad dressing intake [g/d]</t>
-  </si>
-  <si>
     <t>MAYONNAISE_150103</t>
   </si>
   <si>
-    <t>Intake of mayonnaise, hollandaise and related sauces [g/d]</t>
-  </si>
-  <si>
     <t>DESSERTSAUCE_150104</t>
   </si>
   <si>
@@ -745,9 +621,6 @@
     <t>CONDIMENTS_1504</t>
   </si>
   <si>
-    <t>Condiments (including table-top formats) intakes [g/d]</t>
-  </si>
-  <si>
     <t>SOUP_BOUILLON_16</t>
   </si>
   <si>
@@ -757,101 +630,227 @@
     <t>SOUP_1601</t>
   </si>
   <si>
-    <t>Intake of soups (ready-to-eat) [g/d]</t>
-  </si>
-  <si>
     <t>BOUILLON_1602</t>
   </si>
   <si>
+    <t>MISCELLANEOUS_17</t>
+  </si>
+  <si>
+    <t>Intake of miscellaneous [g/d]</t>
+  </si>
+  <si>
+    <t>VEG_DISHES_1700</t>
+  </si>
+  <si>
+    <t>Intake of vegetarian products and dishes [g/d]</t>
+  </si>
+  <si>
+    <t>SOY_PROD_1701</t>
+  </si>
+  <si>
+    <t>DIET_PROD_1702</t>
+  </si>
+  <si>
+    <t>Intake of food for weight reduction [g/d]</t>
+  </si>
+  <si>
+    <t>ART_SWEETENER_170201</t>
+  </si>
+  <si>
+    <t>Intake of artificial sweeteners (e.g., aspartam, saccharine) [g/d]</t>
+  </si>
+  <si>
+    <t>SNACKS_1703</t>
+  </si>
+  <si>
+    <t>Intake of snacks other than chips and similar [g/d]</t>
+  </si>
+  <si>
+    <t>AMPHIBIANS_1704</t>
+  </si>
+  <si>
+    <t>intake of amphibians, reptiles, snails, insects [g/d]</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>primary school completed</t>
+  </si>
+  <si>
+    <t>technical/professional school completed</t>
+  </si>
+  <si>
+    <t>secondary school</t>
+  </si>
+  <si>
+    <t>longer education (incl. university)</t>
+  </si>
+  <si>
+    <t>not specified</t>
+  </si>
+  <si>
+    <t>never</t>
+  </si>
+  <si>
+    <t>former</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>Fruiting vegetable intake [g/d]</t>
+  </si>
+  <si>
+    <t>Root and tuber vegetable intake [g/d]</t>
+  </si>
+  <si>
+    <t>Mushroom intake [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of legumes with pod [g/d]</t>
+  </si>
+  <si>
+    <t>Bulb vegetables (onions, garlic) intake [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of stems/stalks eaten as vegetables [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of mixed vegetable salad or mixed green salad [g/d]</t>
+  </si>
+  <si>
+    <t>Intake fresh seeds (without pod) from legumes (beans, peas etc.) [g/d]</t>
+  </si>
+  <si>
+    <t>Total fruit intake [g/d]</t>
+  </si>
+  <si>
+    <t>Total legumes intake [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of fresh fruits [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of tree nuts and seeds [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of olives [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of fermented milk products [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of pastas and rice [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of bread and bread products [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of breakfast cereals [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of lamb and sheep meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of horse meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of goat meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of poultry meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of other poultry meat[g/d]</t>
+  </si>
+  <si>
+    <t>Intake of chicken meat[g/d]</t>
+  </si>
+  <si>
+    <t>Intake of turkey meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of duck meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of goose meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of rabbit meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of game [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of fish and seafood and products thereof [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of processed fish[g/d]</t>
+  </si>
+  <si>
+    <t>Intake of eggs [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of animal and vegetable fats and oils [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of vegetable fats and oils [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of fats and oils from marine sources [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of animal fats (processed fat from animal tissue) [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of spoonable desserts and ice creams [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of fruit and vegetable juices [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of soft drinks [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of fortified/liqueur wine [g/d]</t>
+  </si>
+  <si>
+    <t>Dressing intake [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of mayonnaise [g/d]</t>
+  </si>
+  <si>
+    <t>Condiments intakes [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of soups [g/d]</t>
+  </si>
+  <si>
     <t>Intake of mixed vegetables soup, clear
-Meat soup, clear [g/d]</t>
-  </si>
-  <si>
-    <t>MISCELLANEOUS_17</t>
-  </si>
-  <si>
-    <t>Intake of miscellaneous [g/d]</t>
-  </si>
-  <si>
-    <t>VEG_DISHES_1700</t>
-  </si>
-  <si>
-    <t>Intake of vegetarian products and dishes [g/d]</t>
-  </si>
-  <si>
-    <t>SOY_PROD_1701</t>
-  </si>
-  <si>
-    <t>Intake of Soya drink and yoghurt [g/d]</t>
-  </si>
-  <si>
-    <t>DIET_PROD_1702</t>
-  </si>
-  <si>
-    <t>Intake of food for weight reduction [g/d]</t>
-  </si>
-  <si>
-    <t>ART_SWEETENER_170201</t>
-  </si>
-  <si>
-    <t>Intake of artificial sweeteners (e.g., aspartam, saccharine) [g/d]</t>
-  </si>
-  <si>
-    <t>SNACKS_1703</t>
-  </si>
-  <si>
-    <t>Intake of snacks other than chips and similar [g/d]</t>
-  </si>
-  <si>
-    <t>AMPHIBIANS_1704</t>
-  </si>
-  <si>
-    <t>intake of amphibians, reptiles, snails, insects [g/d]</t>
-  </si>
-  <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>primary school completed</t>
-  </si>
-  <si>
-    <t>technical/professional school completed</t>
-  </si>
-  <si>
-    <t>secondary school</t>
-  </si>
-  <si>
-    <t>longer education (incl. university)</t>
-  </si>
-  <si>
-    <t>not specified</t>
-  </si>
-  <si>
-    <t>never</t>
-  </si>
-  <si>
-    <t>former</t>
-  </si>
-  <si>
-    <t>current</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>label</t>
+meat soup, clear [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of soy products [g/d]</t>
   </si>
 </sst>
 </file>
@@ -1371,20 +1370,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="34.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="4"/>
+    <col min="2" max="2" width="34.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.88671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1392,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>272</v>
+        <v>227</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -1408,7 +1407,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1432,7 +1431,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1447,7 +1446,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1462,7 +1461,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1477,7 +1476,7 @@
       </c>
       <c r="E5" s="16"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1492,7 +1491,7 @@
       </c>
       <c r="E6" s="17"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1507,7 +1506,7 @@
       </c>
       <c r="E7" s="17"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1522,7 +1521,7 @@
       </c>
       <c r="E8" s="17"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1537,7 +1536,7 @@
       </c>
       <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1552,7 +1551,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1567,7 +1566,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1582,7 +1581,7 @@
       </c>
       <c r="E12" s="26"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1597,7 +1596,7 @@
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1605,1591 +1604,1591 @@
         <v>30</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>228</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="25"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>35</v>
-      </c>
       <c r="D16" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>37</v>
+        <v>230</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>39</v>
+        <v>231</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>41</v>
+        <v>232</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>43</v>
+        <v>233</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>45</v>
+        <v>234</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>47</v>
+        <v>237</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>49</v>
+        <v>235</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>51</v>
+        <v>236</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>53</v>
+        <v>238</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>55</v>
+        <v>239</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>59</v>
+        <v>240</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>67</v>
+        <v>241</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>87</v>
+        <v>242</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>89</v>
+        <v>243</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>95</v>
+        <v>244</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>47</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="C50" s="27" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>50</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>51</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C52" s="27" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C53" s="27" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C54" s="27" t="s">
-        <v>111</v>
+        <v>245</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C55" s="27" t="s">
-        <v>113</v>
+        <v>246</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="C56" s="27" t="s">
-        <v>115</v>
+        <v>247</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C57" s="27" t="s">
-        <v>117</v>
+        <v>248</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>119</v>
+        <v>249</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="C59" s="27" t="s">
-        <v>121</v>
+        <v>250</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="C60" s="27" t="s">
-        <v>123</v>
+        <v>251</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C61" s="27" t="s">
-        <v>125</v>
+        <v>252</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="C62" s="27" t="s">
-        <v>127</v>
+        <v>253</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>62</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C63" s="27" t="s">
-        <v>129</v>
+        <v>254</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>63</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="C64" s="27" t="s">
-        <v>131</v>
+        <v>255</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>64</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="C65" s="27" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>65</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="C66" s="27" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>66</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="C67" s="27" t="s">
-        <v>137</v>
+        <v>256</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="C68" s="27" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>68</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
       <c r="C69" s="27" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>69</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="C70" s="27" t="s">
-        <v>143</v>
+        <v>257</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>70</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="C72" s="27" t="s">
-        <v>147</v>
+        <v>258</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="C73" s="27" t="s">
-        <v>149</v>
+        <v>259</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="C74" s="27" t="s">
-        <v>151</v>
+        <v>260</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="C75" s="27" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>75</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="C76" s="27" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="C77" s="27" t="s">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>77</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="C78" s="27" t="s">
-        <v>159</v>
+        <v>261</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>78</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="C79" s="27" t="s">
-        <v>161</v>
+        <v>262</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>79</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C80" s="27" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>80</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="C81" s="27" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>81</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="C82" s="27" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>82</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="C83" s="27" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>83</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="C85" s="27" t="s">
-        <v>173</v>
+        <v>263</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>174</v>
+        <v>138</v>
       </c>
       <c r="C86" s="27" t="s">
-        <v>175</v>
+        <v>139</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>86</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
       <c r="C87" s="27" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>87</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>88</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="C89" s="27" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="C90" s="27" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>90</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="C91" s="27" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>91</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="C92" s="27" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>92</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
       <c r="C93" s="27" t="s">
-        <v>189</v>
+        <v>264</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="C94" s="27" t="s">
-        <v>191</v>
+        <v>265</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>94</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="C95" s="27" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>95</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="C96" s="27" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
       <c r="C97" s="27" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>97</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="C98" s="27" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>98</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="C99" s="27" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>99</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="C100" s="27" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>100</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>204</v>
+        <v>166</v>
       </c>
       <c r="C101" s="27" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="C102" s="27" t="s">
-        <v>207</v>
+        <v>169</v>
       </c>
       <c r="D102" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="C103" s="27" t="s">
-        <v>209</v>
+        <v>266</v>
       </c>
       <c r="D103" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="C104" s="27" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="C105" s="27" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>105</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="C106" s="27" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>106</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="C107" s="27" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="D107" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>107</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>218</v>
+        <v>179</v>
       </c>
       <c r="C108" s="27" t="s">
-        <v>219</v>
+        <v>180</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
         <v>108</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="C109" s="27" t="s">
-        <v>221</v>
+        <v>182</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>109</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="C110" s="27" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="D110" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
         <v>110</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="C111" s="27" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
       <c r="D111" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>111</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="C112" s="27" t="s">
-        <v>227</v>
+        <v>267</v>
       </c>
       <c r="D112" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>112</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
       <c r="C113" s="27" t="s">
-        <v>229</v>
+        <v>268</v>
       </c>
       <c r="D113" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
         <v>113</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>230</v>
+        <v>189</v>
       </c>
       <c r="C114" s="27" t="s">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="D114" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
         <v>114</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>232</v>
+        <v>191</v>
       </c>
       <c r="C115" s="27" t="s">
-        <v>233</v>
+        <v>192</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>115</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>234</v>
+        <v>193</v>
       </c>
       <c r="C116" s="27" t="s">
-        <v>235</v>
+        <v>194</v>
       </c>
       <c r="D116" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="4">
         <v>116</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>236</v>
+        <v>195</v>
       </c>
       <c r="C117" s="27" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="4">
         <v>117</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>238</v>
+        <v>196</v>
       </c>
       <c r="C118" s="27" t="s">
-        <v>239</v>
+        <v>197</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>118</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>240</v>
+        <v>198</v>
       </c>
       <c r="C119" s="27" t="s">
-        <v>241</v>
+        <v>270</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="4">
         <v>119</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>242</v>
+        <v>199</v>
       </c>
       <c r="C120" s="27" t="s">
-        <v>243</v>
+        <v>271</v>
       </c>
       <c r="D120" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="4">
         <v>120</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>244</v>
+        <v>200</v>
       </c>
       <c r="C121" s="27" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>121</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>246</v>
+        <v>202</v>
       </c>
       <c r="C122" s="27" t="s">
-        <v>247</v>
+        <v>203</v>
       </c>
       <c r="D122" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="4">
         <v>122</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>248</v>
+        <v>204</v>
       </c>
       <c r="C123" s="27" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
       <c r="D123" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="4">
         <v>123</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
       <c r="C124" s="27" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
       <c r="D124" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>124</v>
       </c>
       <c r="B125" s="7" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="C125" s="27" t="s">
-        <v>253</v>
+        <v>208</v>
       </c>
       <c r="D125" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="4">
         <v>125</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>254</v>
+        <v>209</v>
       </c>
       <c r="C126" s="27" t="s">
-        <v>255</v>
+        <v>210</v>
       </c>
       <c r="D126" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="4">
         <v>126</v>
       </c>
       <c r="B127" s="7" t="s">
-        <v>256</v>
+        <v>211</v>
       </c>
       <c r="C127" s="27" t="s">
-        <v>257</v>
+        <v>212</v>
       </c>
       <c r="D127" s="4" t="s">
         <v>15</v>
@@ -3220,15 +3219,15 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -3237,15 +3236,15 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3253,12 +3252,12 @@
       <c r="G2" s="5"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>261</v>
+        <v>216</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3267,12 +3266,12 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>262</v>
+        <v>217</v>
       </c>
       <c r="C4" s="11">
         <v>0</v>
@@ -3281,12 +3280,12 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="C5" s="11">
         <v>1</v>
@@ -3295,12 +3294,12 @@
       <c r="G5" s="16"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="C6" s="11">
         <v>2</v>
@@ -3309,12 +3308,12 @@
       <c r="G6" s="4"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="C7" s="11">
         <v>3</v>
@@ -3323,12 +3322,12 @@
       <c r="G7" s="16"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="C8" s="11">
         <v>4</v>
@@ -3337,24 +3336,24 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>267</v>
+        <v>222</v>
       </c>
       <c r="C9" s="11">
         <v>5</v>
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>268</v>
+        <v>223</v>
       </c>
       <c r="C10" s="11">
         <v>1</v>
@@ -3363,12 +3362,12 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="C11" s="11">
         <v>2</v>
@@ -3377,12 +3376,12 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="C12" s="11">
         <v>3</v>
@@ -3391,12 +3390,12 @@
       <c r="G12" s="4"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>271</v>
+        <v>226</v>
       </c>
       <c r="C13" s="11">
         <v>4</v>
@@ -3405,7 +3404,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -3413,252 +3412,252 @@
       <c r="G14" s="16"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="3"/>
       <c r="C15" s="11"/>
       <c r="G15" s="16"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="G16" s="16"/>
       <c r="H16" s="20"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="G17" s="16"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="3"/>
       <c r="C21" s="11"/>
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="3"/>
       <c r="C23" s="11"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="3"/>
       <c r="C25" s="11"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="3"/>
       <c r="C27" s="11"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
       <c r="G28" s="16"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="3"/>
       <c r="C29" s="11"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="C31" s="11"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="C33" s="11"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="11"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="11"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="C39" s="11"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="C41" s="11"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="11"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="10"/>
       <c r="C44" s="11"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="11"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="3"/>
       <c r="C47" s="11"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="4"/>
       <c r="B48" s="10"/>
       <c r="C48" s="11"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
       <c r="B49" s="3"/>
       <c r="C49" s="11"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="10"/>
       <c r="C50" s="11"/>
       <c r="E50" s="16"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="3"/>
       <c r="C51" s="11"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="3"/>
       <c r="C53" s="11"/>
       <c r="E53" s="22"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="4"/>
       <c r="B54" s="10"/>
       <c r="C54" s="11"/>
       <c r="E54" s="22"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="4"/>
       <c r="B55" s="3"/>
       <c r="C55" s="11"/>
       <c r="E55" s="16"/>
       <c r="F55" s="23"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="15"/>
       <c r="B56" s="10"/>
       <c r="C56" s="11"/>
@@ -3667,7 +3666,7 @@
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="15"/>
       <c r="B57" s="3"/>
       <c r="C57" s="11"/>
@@ -3676,7 +3675,7 @@
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
       <c r="B58" s="10"/>
       <c r="C58" s="11"/>
@@ -3685,7 +3684,7 @@
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="12"/>
       <c r="B59" s="3"/>
       <c r="C59" s="11"/>
@@ -3694,7 +3693,7 @@
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="10"/>
       <c r="C60" s="11"/>
@@ -3703,7 +3702,7 @@
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="3"/>
       <c r="C61" s="11"/>
@@ -3712,7 +3711,7 @@
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="10"/>
       <c r="C62" s="11"/>
@@ -3721,7 +3720,7 @@
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="3"/>
       <c r="C63" s="11"/>
@@ -3730,7 +3729,7 @@
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
     </row>
-    <row r="64" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="10"/>
       <c r="C64" s="11"/>
@@ -3739,7 +3738,7 @@
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="3"/>
       <c r="C65" s="11"/>
@@ -3748,7 +3747,7 @@
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="10"/>
       <c r="C66" s="11"/>
@@ -3757,7 +3756,7 @@
       <c r="G66" s="7"/>
       <c r="H66" s="7"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="3"/>
       <c r="C67" s="11"/>
@@ -3766,7 +3765,7 @@
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="10"/>
       <c r="C68" s="11"/>
@@ -3775,7 +3774,7 @@
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="3"/>
       <c r="C69" s="11"/>
@@ -3784,7 +3783,7 @@
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
@@ -3793,7 +3792,7 @@
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="13"/>
       <c r="B71" s="3"/>
       <c r="C71" s="11"/>
@@ -3802,7 +3801,7 @@
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="10"/>
       <c r="C72" s="11"/>
@@ -3811,7 +3810,7 @@
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="3"/>
       <c r="C73" s="11"/>
@@ -3820,7 +3819,7 @@
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="10"/>
       <c r="C74" s="11"/>
@@ -3829,7 +3828,7 @@
       <c r="G74" s="7"/>
       <c r="H74" s="7"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="4"/>
       <c r="B75" s="3"/>
       <c r="C75" s="11"/>
@@ -3838,7 +3837,7 @@
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="10"/>
       <c r="C76" s="11"/>
@@ -3847,88 +3846,88 @@
       <c r="G76" s="7"/>
       <c r="H76" s="7"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="4"/>
       <c r="B77" s="3"/>
       <c r="C77" s="11"/>
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="10"/>
       <c r="C78" s="11"/>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="4"/>
       <c r="B79" s="3"/>
       <c r="C79" s="11"/>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
     </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
     </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G82" s="7"/>
       <c r="H82" s="7"/>
     </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
     </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
     </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
     </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G86" s="7"/>
       <c r="H86" s="7"/>
     </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
     </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G88" s="7"/>
       <c r="H88" s="7"/>
     </row>
-    <row r="89" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
     </row>
-    <row r="90" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G90" s="7"/>
       <c r="H90" s="7"/>
     </row>
-    <row r="91" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
     </row>
-    <row r="92" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G92" s="7"/>
       <c r="H92" s="7"/>
     </row>
-    <row r="93" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
     </row>
-    <row r="94" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G94" s="7"/>
       <c r="H94" s="7"/>
     </row>
-    <row r="95" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
     </row>
@@ -3960,6 +3959,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4200,18 +4211,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
   <ds:schemaRefs>
@@ -4221,6 +4220,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B964A4-BD34-45DC-A0C1-F7E06137407B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4237,15 +4253,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
renamed identifier variable to ID from variable_ID and adjusted correct dataset input for energy
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC7D6C4C-E9AD-4666-8CA3-100F85AA7ED1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71AD9D3-0584-473B-880A-87FAE80AA677}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,17 +24,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -54,9 +43,6 @@
     <t>valueType</t>
   </si>
   <si>
-    <t>variable_ID</t>
-  </si>
-  <si>
     <t>participant identification number</t>
   </si>
   <si>
@@ -868,6 +854,9 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1371,7 @@
   <dimension ref="A1:N128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,13 +1412,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="1"/>
@@ -1447,13 +1436,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -1462,13 +1451,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="4"/>
     </row>
@@ -1477,13 +1466,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="16"/>
     </row>
@@ -1492,13 +1481,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="17"/>
     </row>
@@ -1507,13 +1496,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="17"/>
     </row>
@@ -1522,13 +1511,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="17"/>
     </row>
@@ -1537,13 +1526,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="17"/>
     </row>
@@ -1552,13 +1541,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="24"/>
     </row>
@@ -1567,13 +1556,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="25"/>
     </row>
@@ -1582,13 +1571,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>27</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="25"/>
     </row>
@@ -1597,13 +1586,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>29</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="26"/>
     </row>
@@ -1612,13 +1601,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="27" t="s">
-        <v>31</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="25"/>
     </row>
@@ -1627,13 +1616,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>33</v>
-      </c>
       <c r="D15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="25"/>
     </row>
@@ -1642,13 +1631,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>35</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="25"/>
     </row>
@@ -1657,13 +1646,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>37</v>
-      </c>
       <c r="D17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,13 +1660,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>39</v>
-      </c>
       <c r="D18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1685,13 +1674,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>41</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1699,13 +1688,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>43</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1713,13 +1702,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>45</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1727,13 +1716,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>47</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1741,13 +1730,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>49</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1755,13 +1744,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="27" t="s">
-        <v>51</v>
-      </c>
       <c r="D24" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1769,13 +1758,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="27" t="s">
-        <v>53</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1783,13 +1772,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>55</v>
-      </c>
       <c r="D26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1797,13 +1786,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="27" t="s">
-        <v>57</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1811,13 +1800,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="27" t="s">
-        <v>59</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1825,13 +1814,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="27" t="s">
-        <v>61</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1839,13 +1828,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="27" t="s">
-        <v>63</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1853,13 +1842,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="27" t="s">
-        <v>65</v>
-      </c>
       <c r="D31" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1867,13 +1856,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="27" t="s">
-        <v>67</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1881,13 +1870,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="27" t="s">
-        <v>69</v>
-      </c>
       <c r="D33" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1895,13 +1884,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="27" t="s">
-        <v>71</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1909,13 +1898,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="27" t="s">
-        <v>73</v>
-      </c>
       <c r="D35" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1923,13 +1912,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="27" t="s">
-        <v>75</v>
-      </c>
       <c r="D36" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1937,13 +1926,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="27" t="s">
-        <v>77</v>
-      </c>
       <c r="D37" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1951,13 +1940,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="27" t="s">
-        <v>79</v>
-      </c>
       <c r="D38" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1965,13 +1954,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="27" t="s">
-        <v>81</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1979,13 +1968,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="27" t="s">
-        <v>83</v>
-      </c>
       <c r="D40" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1993,13 +1982,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="27" t="s">
-        <v>85</v>
-      </c>
       <c r="D41" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2007,13 +1996,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C42" s="27" t="s">
-        <v>87</v>
-      </c>
       <c r="D42" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2021,13 +2010,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="27" t="s">
-        <v>89</v>
-      </c>
       <c r="D43" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2035,13 +2024,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="27" t="s">
-        <v>91</v>
-      </c>
       <c r="D44" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2049,13 +2038,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="27" t="s">
-        <v>93</v>
-      </c>
       <c r="D45" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2063,13 +2052,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="27" t="s">
-        <v>95</v>
-      </c>
       <c r="D46" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2077,13 +2066,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="27" t="s">
-        <v>97</v>
-      </c>
       <c r="D47" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2091,13 +2080,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="27" t="s">
-        <v>99</v>
-      </c>
       <c r="D48" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2105,13 +2094,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="27" t="s">
-        <v>101</v>
-      </c>
       <c r="D49" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2119,13 +2108,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="27" t="s">
-        <v>103</v>
-      </c>
       <c r="D50" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2133,13 +2122,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="27" t="s">
-        <v>105</v>
-      </c>
       <c r="D51" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,13 +2136,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C52" s="27" t="s">
-        <v>107</v>
-      </c>
       <c r="D52" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2161,13 +2150,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="27" t="s">
-        <v>109</v>
-      </c>
       <c r="D53" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2175,13 +2164,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C54" s="27" t="s">
-        <v>111</v>
-      </c>
       <c r="D54" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2189,13 +2178,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="27" t="s">
-        <v>113</v>
-      </c>
       <c r="D55" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2203,13 +2192,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="27" t="s">
-        <v>115</v>
-      </c>
       <c r="D56" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2217,13 +2206,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="27" t="s">
-        <v>117</v>
-      </c>
       <c r="D57" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2231,13 +2220,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="27" t="s">
-        <v>119</v>
-      </c>
       <c r="D58" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2245,13 +2234,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="C59" s="27" t="s">
-        <v>121</v>
-      </c>
       <c r="D59" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2259,13 +2248,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="C60" s="27" t="s">
-        <v>123</v>
-      </c>
       <c r="D60" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,13 +2262,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C61" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="C61" s="27" t="s">
-        <v>125</v>
-      </c>
       <c r="D61" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2287,13 +2276,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="27" t="s">
-        <v>127</v>
-      </c>
       <c r="D62" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2301,13 +2290,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="27" t="s">
-        <v>129</v>
-      </c>
       <c r="D63" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2315,13 +2304,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="C64" s="27" t="s">
-        <v>131</v>
-      </c>
       <c r="D64" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2329,13 +2318,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="27" t="s">
-        <v>133</v>
-      </c>
       <c r="D65" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2343,13 +2332,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C66" s="27" t="s">
-        <v>135</v>
-      </c>
       <c r="D66" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2357,13 +2346,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="C67" s="27" t="s">
-        <v>137</v>
-      </c>
       <c r="D67" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2371,13 +2360,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="27" t="s">
-        <v>139</v>
-      </c>
       <c r="D68" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2385,13 +2374,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C69" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="27" t="s">
-        <v>141</v>
-      </c>
       <c r="D69" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2399,13 +2388,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="C70" s="27" t="s">
-        <v>143</v>
-      </c>
       <c r="D70" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2413,13 +2402,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="C71" s="27" t="s">
-        <v>145</v>
-      </c>
       <c r="D71" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2427,13 +2416,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C72" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="C72" s="27" t="s">
-        <v>147</v>
-      </c>
       <c r="D72" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2441,13 +2430,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C73" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="C73" s="27" t="s">
-        <v>149</v>
-      </c>
       <c r="D73" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2455,13 +2444,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C74" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="C74" s="27" t="s">
-        <v>151</v>
-      </c>
       <c r="D74" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2469,13 +2458,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C75" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="C75" s="27" t="s">
-        <v>153</v>
-      </c>
       <c r="D75" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2483,13 +2472,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="C76" s="27" t="s">
-        <v>155</v>
-      </c>
       <c r="D76" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2497,13 +2486,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="C77" s="27" t="s">
-        <v>157</v>
-      </c>
       <c r="D77" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2511,13 +2500,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C78" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="C78" s="27" t="s">
-        <v>159</v>
-      </c>
       <c r="D78" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2525,13 +2514,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="27" t="s">
-        <v>161</v>
-      </c>
       <c r="D79" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2539,13 +2528,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C80" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="C80" s="27" t="s">
-        <v>163</v>
-      </c>
       <c r="D80" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2553,13 +2542,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C81" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="C81" s="27" t="s">
-        <v>165</v>
-      </c>
       <c r="D81" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2567,13 +2556,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C82" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="C82" s="27" t="s">
-        <v>167</v>
-      </c>
       <c r="D82" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2581,13 +2570,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C83" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="C83" s="27" t="s">
-        <v>169</v>
-      </c>
       <c r="D83" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2595,13 +2584,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C84" s="27" t="s">
         <v>170</v>
       </c>
-      <c r="C84" s="27" t="s">
-        <v>171</v>
-      </c>
       <c r="D84" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2609,13 +2598,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C85" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="C85" s="27" t="s">
-        <v>173</v>
-      </c>
       <c r="D85" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2623,13 +2612,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="C86" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="C86" s="27" t="s">
-        <v>175</v>
-      </c>
       <c r="D86" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2637,13 +2626,13 @@
         <v>86</v>
       </c>
       <c r="B87" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C87" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="C87" s="27" t="s">
-        <v>177</v>
-      </c>
       <c r="D87" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2651,13 +2640,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C88" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="C88" s="27" t="s">
-        <v>179</v>
-      </c>
       <c r="D88" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2665,13 +2654,13 @@
         <v>88</v>
       </c>
       <c r="B89" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C89" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="C89" s="27" t="s">
-        <v>181</v>
-      </c>
       <c r="D89" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2679,13 +2668,13 @@
         <v>89</v>
       </c>
       <c r="B90" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="C90" s="27" t="s">
-        <v>183</v>
-      </c>
       <c r="D90" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2693,13 +2682,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C91" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="C91" s="27" t="s">
-        <v>185</v>
-      </c>
       <c r="D91" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2707,13 +2696,13 @@
         <v>91</v>
       </c>
       <c r="B92" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C92" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="C92" s="27" t="s">
-        <v>187</v>
-      </c>
       <c r="D92" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2721,13 +2710,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="C93" s="27" t="s">
-        <v>189</v>
-      </c>
       <c r="D93" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2735,13 +2724,13 @@
         <v>93</v>
       </c>
       <c r="B94" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C94" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="C94" s="27" t="s">
-        <v>191</v>
-      </c>
       <c r="D94" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2749,13 +2738,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C95" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="C95" s="27" t="s">
-        <v>193</v>
-      </c>
       <c r="D95" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2763,13 +2752,13 @@
         <v>95</v>
       </c>
       <c r="B96" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C96" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="C96" s="27" t="s">
-        <v>195</v>
-      </c>
       <c r="D96" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2777,13 +2766,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C97" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C97" s="27" t="s">
-        <v>197</v>
-      </c>
       <c r="D97" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2791,13 +2780,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C98" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="C98" s="27" t="s">
-        <v>199</v>
-      </c>
       <c r="D98" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2805,13 +2794,13 @@
         <v>98</v>
       </c>
       <c r="B99" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C99" s="27" t="s">
         <v>200</v>
       </c>
-      <c r="C99" s="27" t="s">
-        <v>201</v>
-      </c>
       <c r="D99" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2819,13 +2808,13 @@
         <v>99</v>
       </c>
       <c r="B100" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C100" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="C100" s="27" t="s">
-        <v>203</v>
-      </c>
       <c r="D100" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2833,13 +2822,13 @@
         <v>100</v>
       </c>
       <c r="B101" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C101" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="C101" s="27" t="s">
-        <v>205</v>
-      </c>
       <c r="D101" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2847,13 +2836,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C102" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="C102" s="27" t="s">
-        <v>207</v>
-      </c>
       <c r="D102" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2861,13 +2850,13 @@
         <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C103" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="C103" s="27" t="s">
-        <v>209</v>
-      </c>
       <c r="D103" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2875,13 +2864,13 @@
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C104" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="C104" s="27" t="s">
-        <v>211</v>
-      </c>
       <c r="D104" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2889,13 +2878,13 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C105" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="C105" s="27" t="s">
-        <v>213</v>
-      </c>
       <c r="D105" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2903,13 +2892,13 @@
         <v>105</v>
       </c>
       <c r="B106" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C106" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="C106" s="27" t="s">
-        <v>215</v>
-      </c>
       <c r="D106" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2917,13 +2906,13 @@
         <v>106</v>
       </c>
       <c r="B107" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C107" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="C107" s="27" t="s">
-        <v>217</v>
-      </c>
       <c r="D107" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2931,13 +2920,13 @@
         <v>107</v>
       </c>
       <c r="B108" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C108" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="C108" s="27" t="s">
-        <v>219</v>
-      </c>
       <c r="D108" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2945,13 +2934,13 @@
         <v>108</v>
       </c>
       <c r="B109" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C109" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="C109" s="27" t="s">
-        <v>221</v>
-      </c>
       <c r="D109" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2959,13 +2948,13 @@
         <v>109</v>
       </c>
       <c r="B110" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C110" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="C110" s="27" t="s">
-        <v>223</v>
-      </c>
       <c r="D110" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2973,13 +2962,13 @@
         <v>110</v>
       </c>
       <c r="B111" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C111" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="C111" s="27" t="s">
-        <v>225</v>
-      </c>
       <c r="D111" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2987,13 +2976,13 @@
         <v>111</v>
       </c>
       <c r="B112" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C112" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="C112" s="27" t="s">
-        <v>227</v>
-      </c>
       <c r="D112" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -3001,13 +2990,13 @@
         <v>112</v>
       </c>
       <c r="B113" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C113" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="C113" s="27" t="s">
-        <v>229</v>
-      </c>
       <c r="D113" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3015,13 +3004,13 @@
         <v>113</v>
       </c>
       <c r="B114" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C114" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="C114" s="27" t="s">
-        <v>231</v>
-      </c>
       <c r="D114" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3029,13 +3018,13 @@
         <v>114</v>
       </c>
       <c r="B115" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C115" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="C115" s="27" t="s">
-        <v>233</v>
-      </c>
       <c r="D115" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3043,13 +3032,13 @@
         <v>115</v>
       </c>
       <c r="B116" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C116" s="27" t="s">
         <v>234</v>
       </c>
-      <c r="C116" s="27" t="s">
-        <v>235</v>
-      </c>
       <c r="D116" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3057,13 +3046,13 @@
         <v>116</v>
       </c>
       <c r="B117" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C117" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="C117" s="27" t="s">
-        <v>237</v>
-      </c>
       <c r="D117" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3071,13 +3060,13 @@
         <v>117</v>
       </c>
       <c r="B118" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C118" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="C118" s="27" t="s">
-        <v>239</v>
-      </c>
       <c r="D118" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3085,13 +3074,13 @@
         <v>118</v>
       </c>
       <c r="B119" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="C119" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="C119" s="27" t="s">
-        <v>241</v>
-      </c>
       <c r="D119" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3099,13 +3088,13 @@
         <v>119</v>
       </c>
       <c r="B120" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C120" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="C120" s="27" t="s">
-        <v>243</v>
-      </c>
       <c r="D120" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3113,13 +3102,13 @@
         <v>120</v>
       </c>
       <c r="B121" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C121" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="C121" s="27" t="s">
-        <v>245</v>
-      </c>
       <c r="D121" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3127,13 +3116,13 @@
         <v>121</v>
       </c>
       <c r="B122" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C122" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="C122" s="27" t="s">
-        <v>247</v>
-      </c>
       <c r="D122" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3141,13 +3130,13 @@
         <v>122</v>
       </c>
       <c r="B123" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C123" s="27" t="s">
         <v>248</v>
       </c>
-      <c r="C123" s="27" t="s">
-        <v>249</v>
-      </c>
       <c r="D123" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -3155,13 +3144,13 @@
         <v>123</v>
       </c>
       <c r="B124" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C124" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="C124" s="27" t="s">
-        <v>251</v>
-      </c>
       <c r="D124" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3169,13 +3158,13 @@
         <v>124</v>
       </c>
       <c r="B125" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C125" s="27" t="s">
         <v>252</v>
       </c>
-      <c r="C125" s="27" t="s">
-        <v>253</v>
-      </c>
       <c r="D125" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3183,13 +3172,13 @@
         <v>125</v>
       </c>
       <c r="B126" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C126" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="C126" s="27" t="s">
-        <v>255</v>
-      </c>
       <c r="D126" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3197,13 +3186,13 @@
         <v>126</v>
       </c>
       <c r="B127" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C127" s="27" t="s">
         <v>256</v>
       </c>
-      <c r="C127" s="27" t="s">
-        <v>257</v>
-      </c>
       <c r="D127" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3211,13 +3200,13 @@
         <v>127</v>
       </c>
       <c r="B128" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C128" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="C128" s="27" t="s">
-        <v>259</v>
-      </c>
       <c r="D128" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3253,24 +3242,24 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3280,10 +3269,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3294,10 +3283,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C4" s="11">
         <v>0</v>
@@ -3308,10 +3297,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C5" s="11">
         <v>1</v>
@@ -3322,10 +3311,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C6" s="11">
         <v>2</v>
@@ -3336,10 +3325,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C7" s="11">
         <v>3</v>
@@ -3350,10 +3339,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="11">
         <v>4</v>
@@ -3364,10 +3353,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C9" s="11">
         <v>5</v>
@@ -3376,10 +3365,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C10" s="11">
         <v>1</v>
@@ -3390,10 +3379,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C11" s="11">
         <v>2</v>
@@ -3404,10 +3393,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C12" s="11">
         <v>3</v>
@@ -3418,10 +3407,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C13" s="11">
         <v>4</v>
@@ -4217,15 +4206,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -4235,6 +4215,15 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4257,14 +4246,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4279,4 +4260,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding information on the variable DIETARY_ASSESS_INSTR for Variables and Categories sheet in both P1 and P2 Dataschemas
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E044155E-C8FA-4495-A3D7-15B64425D16A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E663E4B-1709-4616-A837-B0A79D4B2371}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="282">
   <si>
     <t>index</t>
   </si>
@@ -851,6 +851,33 @@
   </si>
   <si>
     <t>Participant identification number</t>
+  </si>
+  <si>
+    <t>DIETARY_ASSESS_INSTR</t>
+  </si>
+  <si>
+    <t>Dietary Assessment Instrument</t>
+  </si>
+  <si>
+    <t>FPQ (Food propensity questionnair without portion sizes)</t>
+  </si>
+  <si>
+    <t>FFQ (Food frequency questionnaire</t>
+  </si>
+  <si>
+    <t>24HDR (24-h dietary recall</t>
+  </si>
+  <si>
+    <t>3_d_FR_w (3-day weighing food record)</t>
+  </si>
+  <si>
+    <t>7_d_FR_w (7-day weighing food record)</t>
+  </si>
+  <si>
+    <t>7_d_FR (7-day  food record; described portion sizes)</t>
+  </si>
+  <si>
+    <t>24HFL_FFQ (24-h short food list combined with FFQ</t>
   </si>
 </sst>
 </file>
@@ -904,9 +931,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -922,7 +949,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1218,21 +1245,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D128"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129:D129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625"/>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375"/>
+    <col min="2" max="2" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1260,7 +1287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1274,7 +1301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1288,7 +1315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1302,7 +1329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1316,7 +1343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1330,7 +1357,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1344,7 +1371,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1358,7 +1385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1372,7 +1399,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1386,7 +1413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1400,7 +1427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1414,7 +1441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1428,7 +1455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1442,7 +1469,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1456,7 +1483,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1470,7 +1497,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1484,7 +1511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1498,7 +1525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1512,7 +1539,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1526,7 +1553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1540,7 +1567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1554,7 +1581,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1568,7 +1595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1582,7 +1609,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1596,7 +1623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1610,7 +1637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1624,7 +1651,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1638,7 +1665,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1652,7 +1679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1666,7 +1693,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1680,7 +1707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1694,7 +1721,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1708,7 +1735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1722,7 +1749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1736,7 +1763,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1750,7 +1777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1764,7 +1791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1778,7 +1805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1792,7 +1819,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1806,7 +1833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1820,7 +1847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1834,7 +1861,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1848,7 +1875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1862,7 +1889,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1876,7 +1903,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1890,7 +1917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1904,7 +1931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1918,7 +1945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1932,7 +1959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1946,7 +1973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1960,7 +1987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1974,7 +2001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1988,7 +2015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2002,7 +2029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2016,7 +2043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2030,7 +2057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2044,7 +2071,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2058,7 +2085,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2072,7 +2099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2086,7 +2113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2100,7 +2127,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2114,7 +2141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2128,7 +2155,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2142,7 +2169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2156,7 +2183,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2170,7 +2197,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2184,7 +2211,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2198,7 +2225,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2212,7 +2239,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2226,7 +2253,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2240,7 +2267,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2254,7 +2281,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2268,7 +2295,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2282,7 +2309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2296,7 +2323,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2310,7 +2337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2324,7 +2351,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2338,7 +2365,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2352,7 +2379,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2366,7 +2393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2380,7 +2407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2394,7 +2421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2408,7 +2435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2422,7 +2449,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2436,7 +2463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2450,7 +2477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2464,7 +2491,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2478,7 +2505,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2492,7 +2519,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2506,7 +2533,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2520,7 +2547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2534,7 +2561,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2548,7 +2575,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2562,7 +2589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2576,7 +2603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2590,7 +2617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2604,7 +2631,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2618,7 +2645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2632,7 +2659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2646,7 +2673,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2660,7 +2687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2674,7 +2701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2688,7 +2715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2702,7 +2729,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2716,7 +2743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2730,7 +2757,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2744,7 +2771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2758,7 +2785,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2772,7 +2799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2786,7 +2813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2800,7 +2827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2814,7 +2841,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2828,7 +2855,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2842,7 +2869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2856,7 +2883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2870,7 +2897,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2884,7 +2911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2898,7 +2925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2912,7 +2939,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2926,7 +2953,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2940,7 +2967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2954,7 +2981,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2968,7 +2995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2982,7 +3009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2996,7 +3023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3010,7 +3037,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3022,6 +3049,20 @@
       </c>
       <c r="D128" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>273</v>
+      </c>
+      <c r="C129" t="s">
+        <v>274</v>
+      </c>
+      <c r="D129" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3042,17 +3083,17 @@
   <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A14" sqref="A14:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>258</v>
       </c>
@@ -3063,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3074,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3085,7 +3126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3096,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3107,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3118,7 +3159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3129,7 +3170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3140,7 +3181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3151,7 +3192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3162,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3173,7 +3214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3184,7 +3225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -3195,7 +3236,84 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14" t="s">
+        <v>275</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>273</v>
+      </c>
+      <c r="B15" t="s">
+        <v>276</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16" t="s">
+        <v>277</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>273</v>
+      </c>
+      <c r="B17" t="s">
+        <v>278</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>273</v>
+      </c>
+      <c r="B18" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B19" t="s">
+        <v>279</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" ht="14.1" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{85760D7C-312A-4647-B300-A227B229A527}">
@@ -3222,6 +3340,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -3462,15 +3589,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
   <ds:schemaRefs>
@@ -3489,6 +3607,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B964A4-BD34-45DC-A0C1-F7E06137407B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3505,12 +3631,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding the dieatary assessment instrument and doing a final check
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E663E4B-1709-4616-A837-B0A79D4B2371}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470C8956-A43D-453C-A708-4BB091B4DC0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -1247,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129:D129"/>
+    <sheetView topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3082,8 +3082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3328,27 +3328,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -3589,32 +3568,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B964A4-BD34-45DC-A0C1-F7E06137407B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3631,4 +3606,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
small changes to the Description of the Variables / Categories in Dataschema_P1
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470C8956-A43D-453C-A708-4BB091B4DC0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B351634-6432-4E17-B921-CC7B0B1FFC6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>BMI</t>
   </si>
   <si>
-    <t>Body Mass index at baseline</t>
-  </si>
-  <si>
     <t>ENERGY</t>
   </si>
   <si>
@@ -244,16 +241,9 @@
     <t>CHEESE_0505</t>
   </si>
   <si>
-    <t>Intake of Cheese [g/d]</t>
-  </si>
-  <si>
     <t>DAIRYDESSERT_0506</t>
   </si>
   <si>
-    <t>Intake of dairy dessert and similar
-Starchy pudding [g/d]</t>
-  </si>
-  <si>
     <t>CREAM_PROD_0507</t>
   </si>
   <si>
@@ -269,9 +259,6 @@
     <t>NONDAIRYCREAM_050702</t>
   </si>
   <si>
-    <t>Intake of Imitation cream, non-dairy coffee creamers and dairy imitates other than milk [g/d]</t>
-  </si>
-  <si>
     <t>MILK_FOR_COFFEE_0508</t>
   </si>
   <si>
@@ -281,10 +268,6 @@
     <t>CEREAL_PROD_06</t>
   </si>
   <si>
-    <t>Intake of cereals and cereal primary derivatives
-Cereal grains (and cereal-like grains) [g/d]</t>
-  </si>
-  <si>
     <t>FLOUR_FLAKES_0601</t>
   </si>
   <si>
@@ -330,9 +313,6 @@
     <t>DOUGH_PASTRY_0606</t>
   </si>
   <si>
-    <t>Intake of fine bakery wares [g/d]</t>
-  </si>
-  <si>
     <t>MEAT_PROD_07</t>
   </si>
   <si>
@@ -390,15 +370,9 @@
     <t>OTHERPOULTRY_070200</t>
   </si>
   <si>
-    <t>Intake of other poultry meat[g/d]</t>
-  </si>
-  <si>
     <t>CHICKEN_070201</t>
   </si>
   <si>
-    <t>Intake of chicken meat[g/d]</t>
-  </si>
-  <si>
     <t>TURKEY_070202</t>
   </si>
   <si>
@@ -450,9 +424,6 @@
     <t>FISH_0801</t>
   </si>
   <si>
-    <t>Intake of Fish (meat) [g/d]</t>
-  </si>
-  <si>
     <t>CRUSTACEANS_0802</t>
   </si>
   <si>
@@ -462,9 +433,6 @@
     <t>FISH_PROD_0803</t>
   </si>
   <si>
-    <t>Intake of processed fish[g/d]</t>
-  </si>
-  <si>
     <t>EGG_PROD_09</t>
   </si>
   <si>
@@ -534,9 +502,6 @@
     <t>CHOCOLATE_1102</t>
   </si>
   <si>
-    <t>Intake of chocolate, chocolate products and chocolate coated conectionary [g/d]</t>
-  </si>
-  <si>
     <t>NONCHOC_SWEETS_1103</t>
   </si>
   <si>
@@ -576,9 +541,6 @@
     <t>CAKES_12</t>
   </si>
   <si>
-    <t>Intake of cakes and fine bakery wares [g/d]</t>
-  </si>
-  <si>
     <t>VARPASTRY_1201</t>
   </si>
   <si>
@@ -744,9 +706,6 @@
     <t>CONDIMENTS_1504</t>
   </si>
   <si>
-    <t>Condiments intakes [g/d]</t>
-  </si>
-  <si>
     <t>SOUP_BOUILLON_16</t>
   </si>
   <si>
@@ -762,10 +721,6 @@
     <t>BOUILLON_1602</t>
   </si>
   <si>
-    <t>Intake of mixed vegetables soup, clear
-meat soup, clear [g/d]</t>
-  </si>
-  <si>
     <t>MISCELLANEOUS_17</t>
   </si>
   <si>
@@ -805,9 +760,6 @@
     <t>AMPHIBIANS_1704</t>
   </si>
   <si>
-    <t>intake of amphibians, reptiles, snails, insects [g/d]</t>
-  </si>
-  <si>
     <t>variable</t>
   </si>
   <si>
@@ -865,9 +817,6 @@
     <t>FFQ (Food frequency questionnaire</t>
   </si>
   <si>
-    <t>24HDR (24-h dietary recall</t>
-  </si>
-  <si>
     <t>3_d_FR_w (3-day weighing food record)</t>
   </si>
   <si>
@@ -877,7 +826,55 @@
     <t>7_d_FR (7-day  food record; described portion sizes)</t>
   </si>
   <si>
-    <t>24HFL_FFQ (24-h short food list combined with FFQ</t>
+    <t>Body Mass Index at baseline</t>
+  </si>
+  <si>
+    <t>Intake of cheese [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of dairy dessert and similar starchy pudding [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of imitation cream, non-dairy coffee creamers and dairy imitates other than milk [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of cereals and cereal primary derivatives, cereal grains (and cereal-like grains) [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of fine bakery products [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of other poultry meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of chicken meat [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of fish (meat) [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of processed fish [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of chocolate, chocolate products and chocolate coated confectionary [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of cakes and fine bakery products [g/d]</t>
+  </si>
+  <si>
+    <t>Condiments intake [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of mixed vegetables soup, clear meat soup, clear [g/d]</t>
+  </si>
+  <si>
+    <t>Intake of amphibians, reptiles, snails, insects [g/d]</t>
+  </si>
+  <si>
+    <t>24HDR (24-h dietary recall)</t>
+  </si>
+  <si>
+    <t>24HFL_FFQ (24-h short food list combined with FFQ)</t>
   </si>
 </sst>
 </file>
@@ -927,8 +924,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -1247,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,10 +1276,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -1365,7 +1363,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>265</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -1376,10 +1374,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -1390,10 +1388,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1404,10 +1402,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -1418,10 +1416,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -1432,10 +1430,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -1446,10 +1444,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -1460,10 +1458,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
         <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -1474,10 +1472,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -1488,10 +1486,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>35</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -1502,10 +1500,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
         <v>36</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -1516,10 +1514,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
@@ -1530,10 +1528,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
@@ -1544,10 +1542,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
@@ -1558,10 +1556,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" t="s">
-        <v>45</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
@@ -1572,10 +1570,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
@@ -1586,10 +1584,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
         <v>48</v>
-      </c>
-      <c r="C24" t="s">
-        <v>49</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
@@ -1600,10 +1598,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
         <v>50</v>
-      </c>
-      <c r="C25" t="s">
-        <v>51</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
@@ -1614,10 +1612,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
         <v>52</v>
-      </c>
-      <c r="C26" t="s">
-        <v>53</v>
       </c>
       <c r="D26" t="s">
         <v>13</v>
@@ -1628,10 +1626,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
         <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
       </c>
       <c r="D27" t="s">
         <v>13</v>
@@ -1642,10 +1640,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
         <v>56</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
@@ -1656,10 +1654,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
         <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>59</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
@@ -1670,10 +1668,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
         <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>61</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
@@ -1684,10 +1682,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
         <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>63</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -1698,10 +1696,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" t="s">
-        <v>65</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -1712,10 +1710,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
         <v>66</v>
-      </c>
-      <c r="C33" t="s">
-        <v>67</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
@@ -1726,10 +1724,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" t="s">
         <v>68</v>
-      </c>
-      <c r="C34" t="s">
-        <v>69</v>
       </c>
       <c r="D34" t="s">
         <v>13</v>
@@ -1740,10 +1738,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>266</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -1754,10 +1752,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>267</v>
       </c>
       <c r="D36" t="s">
         <v>13</v>
@@ -1768,10 +1766,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D37" t="s">
         <v>13</v>
@@ -1782,10 +1780,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D38" t="s">
         <v>13</v>
@@ -1796,10 +1794,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>268</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
@@ -1810,10 +1808,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -1824,10 +1822,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>269</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
@@ -1838,10 +1836,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
         <v>13</v>
@@ -1852,10 +1850,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
         <v>13</v>
@@ -1866,10 +1864,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
@@ -1880,10 +1878,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D45" t="s">
         <v>13</v>
@@ -1894,10 +1892,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>
@@ -1908,10 +1906,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D47" t="s">
         <v>13</v>
@@ -1922,10 +1920,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D48" t="s">
         <v>13</v>
@@ -1936,10 +1934,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
+        <v>270</v>
       </c>
       <c r="D49" t="s">
         <v>13</v>
@@ -1950,10 +1948,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D50" t="s">
         <v>13</v>
@@ -1964,10 +1962,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D51" t="s">
         <v>13</v>
@@ -1978,10 +1976,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D52" t="s">
         <v>13</v>
@@ -1992,10 +1990,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D53" t="s">
         <v>13</v>
@@ -2006,10 +2004,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C54" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D54" t="s">
         <v>13</v>
@@ -2020,10 +2018,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C55" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D55" t="s">
         <v>13</v>
@@ -2034,10 +2032,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C56" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D56" t="s">
         <v>13</v>
@@ -2048,10 +2046,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D57" t="s">
         <v>13</v>
@@ -2062,10 +2060,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C58" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
@@ -2076,10 +2074,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>119</v>
+        <v>271</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
@@ -2090,10 +2088,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C60" t="s">
-        <v>121</v>
+        <v>272</v>
       </c>
       <c r="D60" t="s">
         <v>13</v>
@@ -2104,10 +2102,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C61" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D61" t="s">
         <v>13</v>
@@ -2118,10 +2116,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C62" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D62" t="s">
         <v>13</v>
@@ -2132,10 +2130,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C63" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -2146,10 +2144,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C64" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
@@ -2160,10 +2158,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C65" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D65" t="s">
         <v>13</v>
@@ -2174,10 +2172,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="D66" t="s">
         <v>13</v>
@@ -2188,10 +2186,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C67" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D67" t="s">
         <v>13</v>
@@ -2202,10 +2200,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C68" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="D68" t="s">
         <v>13</v>
@@ -2216,10 +2214,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C69" t="s">
-        <v>139</v>
+        <v>273</v>
       </c>
       <c r="D69" t="s">
         <v>13</v>
@@ -2230,10 +2228,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C70" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D70" t="s">
         <v>13</v>
@@ -2244,10 +2242,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C71" t="s">
-        <v>143</v>
+        <v>274</v>
       </c>
       <c r="D71" t="s">
         <v>13</v>
@@ -2258,10 +2256,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C72" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D72" t="s">
         <v>13</v>
@@ -2272,10 +2270,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C73" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -2286,10 +2284,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C74" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D74" t="s">
         <v>13</v>
@@ -2300,10 +2298,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C75" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D75" t="s">
         <v>13</v>
@@ -2314,10 +2312,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C76" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D76" t="s">
         <v>13</v>
@@ -2328,10 +2326,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C77" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="D77" t="s">
         <v>13</v>
@@ -2342,10 +2340,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D78" t="s">
         <v>13</v>
@@ -2356,10 +2354,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C79" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D79" t="s">
         <v>13</v>
@@ -2370,10 +2368,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C80" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D80" t="s">
         <v>13</v>
@@ -2384,10 +2382,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C81" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D81" t="s">
         <v>13</v>
@@ -2398,10 +2396,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C82" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D82" t="s">
         <v>13</v>
@@ -2412,10 +2410,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C83" t="s">
-        <v>167</v>
+        <v>275</v>
       </c>
       <c r="D83" t="s">
         <v>13</v>
@@ -2426,10 +2424,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C84" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D84" t="s">
         <v>13</v>
@@ -2440,10 +2438,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C85" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D85" t="s">
         <v>13</v>
@@ -2454,10 +2452,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C86" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D86" t="s">
         <v>13</v>
@@ -2468,10 +2466,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C87" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D87" t="s">
         <v>13</v>
@@ -2482,10 +2480,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C88" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D88" t="s">
         <v>13</v>
@@ -2496,10 +2494,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C89" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D89" t="s">
         <v>13</v>
@@ -2510,10 +2508,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C90" t="s">
-        <v>181</v>
+        <v>276</v>
       </c>
       <c r="D90" t="s">
         <v>13</v>
@@ -2524,10 +2522,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C91" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D91" t="s">
         <v>13</v>
@@ -2538,10 +2536,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C92" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D92" t="s">
         <v>13</v>
@@ -2552,10 +2550,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="C93" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D93" t="s">
         <v>13</v>
@@ -2566,10 +2564,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C94" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D94" t="s">
         <v>13</v>
@@ -2580,10 +2578,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C95" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="D95" t="s">
         <v>13</v>
@@ -2594,10 +2592,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C96" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D96" t="s">
         <v>13</v>
@@ -2608,10 +2606,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C97" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="D97" t="s">
         <v>13</v>
@@ -2622,10 +2620,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C98" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="D98" t="s">
         <v>13</v>
@@ -2636,10 +2634,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C99" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D99" t="s">
         <v>13</v>
@@ -2650,10 +2648,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="C100" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D100" t="s">
         <v>13</v>
@@ -2664,10 +2662,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C101" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="D101" t="s">
         <v>13</v>
@@ -2678,10 +2676,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C102" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D102" t="s">
         <v>13</v>
@@ -2692,10 +2690,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C103" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="D103" t="s">
         <v>13</v>
@@ -2706,10 +2704,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="C104" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="D104" t="s">
         <v>13</v>
@@ -2720,10 +2718,10 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C105" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D105" t="s">
         <v>13</v>
@@ -2734,10 +2732,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C106" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D106" t="s">
         <v>13</v>
@@ -2748,10 +2746,10 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="C107" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D107" t="s">
         <v>13</v>
@@ -2762,10 +2760,10 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C108" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="D108" t="s">
         <v>13</v>
@@ -2776,10 +2774,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C109" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="D109" t="s">
         <v>13</v>
@@ -2790,10 +2788,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="C110" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="D110" t="s">
         <v>13</v>
@@ -2804,10 +2802,10 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C111" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="D111" t="s">
         <v>13</v>
@@ -2818,10 +2816,10 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C112" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D112" t="s">
         <v>13</v>
@@ -2832,10 +2830,10 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C113" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="D113" t="s">
         <v>13</v>
@@ -2846,10 +2844,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="C114" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="D114" t="s">
         <v>13</v>
@@ -2860,10 +2858,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C115" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D115" t="s">
         <v>13</v>
@@ -2874,10 +2872,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C116" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="D116" t="s">
         <v>13</v>
@@ -2888,10 +2886,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C117" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D117" t="s">
         <v>13</v>
@@ -2902,10 +2900,10 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="C118" t="s">
-        <v>237</v>
+        <v>277</v>
       </c>
       <c r="D118" t="s">
         <v>13</v>
@@ -2916,10 +2914,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C119" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="D119" t="s">
         <v>13</v>
@@ -2930,10 +2928,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C120" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="D120" t="s">
         <v>13</v>
@@ -2944,10 +2942,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C121" t="s">
-        <v>243</v>
+        <v>278</v>
       </c>
       <c r="D121" t="s">
         <v>13</v>
@@ -2958,10 +2956,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="C122" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="D122" t="s">
         <v>13</v>
@@ -2972,10 +2970,10 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C123" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="D123" t="s">
         <v>13</v>
@@ -2986,10 +2984,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="C124" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="D124" t="s">
         <v>13</v>
@@ -3000,10 +2998,10 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="C125" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="D125" t="s">
         <v>13</v>
@@ -3014,10 +3012,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="C126" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="D126" t="s">
         <v>13</v>
@@ -3028,10 +3026,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="C127" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="D127" t="s">
         <v>13</v>
@@ -3042,10 +3040,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="C128" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D128" t="s">
         <v>13</v>
@@ -3056,10 +3054,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="C129" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D129" t="s">
         <v>4</v>
@@ -3082,20 +3080,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3109,7 +3107,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3120,7 +3118,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3131,7 +3129,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3142,7 +3140,7 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3153,7 +3151,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3164,7 +3162,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -3175,7 +3173,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3186,7 +3184,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -3197,7 +3195,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3208,7 +3206,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -3219,7 +3217,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -3230,7 +3228,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -3238,10 +3236,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B14" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -3249,10 +3247,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B15" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3260,10 +3258,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B16" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3271,10 +3269,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B17" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -3282,10 +3280,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B18" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -3293,10 +3291,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B19" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -3304,7 +3302,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B20" t="s">
         <v>281</v>
@@ -3569,15 +3567,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -3587,6 +3576,15 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3609,14 +3607,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -3631,4 +3621,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
final label editing of P1 in Dataschema and DPE's
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B351634-6432-4E17-B921-CC7B0B1FFC6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7218085F-AECE-45CB-A767-E0DA2D98D424}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -865,9 +865,6 @@
     <t>Condiments intake [g/d]</t>
   </si>
   <si>
-    <t>Intake of mixed vegetables soup, clear meat soup, clear [g/d]</t>
-  </si>
-  <si>
     <t>Intake of amphibians, reptiles, snails, insects [g/d]</t>
   </si>
   <si>
@@ -875,6 +872,9 @@
   </si>
   <si>
     <t>24HFL_FFQ (24-h short food list combined with FFQ)</t>
+  </si>
+  <si>
+    <t>Intake of mixed vegetables soup, clear meat soup [g/d]</t>
   </si>
 </sst>
 </file>
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2945,7 +2945,7 @@
         <v>229</v>
       </c>
       <c r="C121" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D121" t="s">
         <v>13</v>
@@ -3043,7 +3043,7 @@
         <v>242</v>
       </c>
       <c r="C128" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D128" t="s">
         <v>13</v>
@@ -3080,7 +3080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -3261,7 +3261,7 @@
         <v>258</v>
       </c>
       <c r="B16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3305,7 +3305,7 @@
         <v>258</v>
       </c>
       <c r="B20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C20">
         <v>6</v>
@@ -3567,6 +3567,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -3576,15 +3585,6 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3607,6 +3607,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -3621,12 +3629,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- added a missing bracket in label description of one category for dietary instruments
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7218085F-AECE-45CB-A767-E0DA2D98D424}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225FEBFB-30B3-4648-991B-2DFD4A3548F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -814,9 +814,6 @@
     <t>FPQ (Food propensity questionnair without portion sizes)</t>
   </si>
   <si>
-    <t>FFQ (Food frequency questionnaire</t>
-  </si>
-  <si>
     <t>3_d_FR_w (3-day weighing food record)</t>
   </si>
   <si>
@@ -875,6 +872,9 @@
   </si>
   <si>
     <t>Intake of mixed vegetables soup, clear meat soup [g/d]</t>
+  </si>
+  <si>
+    <t>FFQ (Food frequency questionnaire)</t>
   </si>
 </sst>
 </file>
@@ -1245,19 +1245,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375"/>
-    <col min="2" max="2" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1363,13 +1363,13 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1741,13 +1741,13 @@
         <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1755,13 +1755,13 @@
         <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1797,13 +1797,13 @@
         <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D39" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1825,13 +1825,13 @@
         <v>78</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1937,13 +1937,13 @@
         <v>93</v>
       </c>
       <c r="C49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D49" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2077,13 +2077,13 @@
         <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D59" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2091,13 +2091,13 @@
         <v>113</v>
       </c>
       <c r="C60" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D60" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2217,13 +2217,13 @@
         <v>130</v>
       </c>
       <c r="C69" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D69" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2245,13 +2245,13 @@
         <v>133</v>
       </c>
       <c r="C71" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D71" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2413,13 +2413,13 @@
         <v>156</v>
       </c>
       <c r="C83" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D83" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2511,13 +2511,13 @@
         <v>169</v>
       </c>
       <c r="C90" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D90" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2573,7 +2573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2811,7 +2811,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2903,13 +2903,13 @@
         <v>224</v>
       </c>
       <c r="C118" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D118" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2945,13 +2945,13 @@
         <v>229</v>
       </c>
       <c r="C121" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D121" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3043,13 +3043,13 @@
         <v>242</v>
       </c>
       <c r="C128" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D128" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3080,18 +3080,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>243</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>258</v>
       </c>
@@ -3245,73 +3245,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>258</v>
       </c>
       <c r="B15" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>258</v>
       </c>
       <c r="B16" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>258</v>
       </c>
       <c r="B17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>258</v>
       </c>
       <c r="B18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>258</v>
       </c>
       <c r="B19" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C19">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>258</v>
       </c>
       <c r="B20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
     </row>
-    <row r="64" ht="14.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{85760D7C-312A-4647-B300-A227B229A527}">
@@ -3567,15 +3567,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -3585,6 +3576,15 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3607,14 +3607,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -3629,4 +3621,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Dataschema P1 to include units in labels for AGE_BASE, BMI, TOT_PA_QX like Dataschema P2
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225FEBFB-30B3-4648-991B-2DFD4A3548F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF108BD9-EC6D-4B81-9906-F93C9804C1FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -55,9 +55,6 @@
     <t>AGE_BASE</t>
   </si>
   <si>
-    <t>Age at exposure measure</t>
-  </si>
-  <si>
     <t>EDU_LEVEL</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>TOT_PA_QX</t>
   </si>
   <si>
-    <t>Physical activity from questionnaire data</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
@@ -823,9 +817,6 @@
     <t>7_d_FR (7-day  food record; described portion sizes)</t>
   </si>
   <si>
-    <t>Body Mass Index at baseline</t>
-  </si>
-  <si>
     <t>Intake of cheese [g/d]</t>
   </si>
   <si>
@@ -875,6 +866,15 @@
   </si>
   <si>
     <t>FFQ (Food frequency questionnaire)</t>
+  </si>
+  <si>
+    <t>Age at exposure measure [years]</t>
+  </si>
+  <si>
+    <t>Physical activity from questionnaire data [MET-hr/day]</t>
+  </si>
+  <si>
+    <t>Body Mass Index at baseline [kg/m²]</t>
   </si>
 </sst>
 </file>
@@ -929,9 +929,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -947,7 +947,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1245,15 +1245,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625"/>
     <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="138.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1276,10 +1276,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -1307,10 +1307,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>279</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1318,10 +1318,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -1332,13 +1332,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>280</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,10 +1346,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1360,13 +1360,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>264</v>
+        <v>281</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1374,13 +1374,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1388,13 +1388,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,13 +1402,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1416,13 +1416,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,13 +1430,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,13 +1444,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,13 +1458,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,13 +1472,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,13 +1486,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1500,13 +1500,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1514,13 +1514,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1528,13 +1528,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1542,13 +1542,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1556,13 +1556,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,13 +1570,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1584,13 +1584,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1598,13 +1598,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1612,13 +1612,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1626,13 +1626,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1640,13 +1640,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1654,13 +1654,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1668,13 +1668,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1682,13 +1682,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1696,13 +1696,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1710,13 +1710,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1724,13 +1724,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1738,13 +1738,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1752,13 +1752,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1766,13 +1766,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1780,13 +1780,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1794,13 +1794,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,13 +1808,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1822,13 +1822,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1836,13 +1836,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,13 +1850,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1864,13 +1864,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1878,13 +1878,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1892,13 +1892,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,13 +1906,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1920,13 +1920,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C48" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1934,13 +1934,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1948,13 +1948,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1962,13 +1962,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,13 +1976,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,13 +1990,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2004,13 +2004,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D54" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2018,13 +2018,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C55" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2032,13 +2032,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2046,13 +2046,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,13 +2060,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C58" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,13 +2074,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C59" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2088,13 +2088,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C60" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D60" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2102,13 +2102,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2116,13 +2116,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C62" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2130,13 +2130,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2144,13 +2144,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2158,13 +2158,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C65" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D65" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2172,13 +2172,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C66" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D66" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,13 +2186,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C67" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D67" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2200,13 +2200,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C68" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D68" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2214,13 +2214,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D69" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2228,13 +2228,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C70" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D70" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2242,13 +2242,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D71" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2256,13 +2256,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C72" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D72" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2270,13 +2270,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C73" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D73" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2284,13 +2284,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C74" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D74" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2298,13 +2298,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C75" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D75" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2312,13 +2312,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D76" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2326,13 +2326,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C77" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D77" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2340,13 +2340,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C78" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D78" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2354,13 +2354,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C79" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D79" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2368,13 +2368,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C80" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D80" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2382,13 +2382,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C81" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2396,13 +2396,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C82" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D82" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2410,13 +2410,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C83" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D83" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2424,13 +2424,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C84" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D84" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2438,13 +2438,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C85" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D85" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2452,13 +2452,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C86" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D86" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2466,13 +2466,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C87" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D87" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2480,13 +2480,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C88" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D88" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2494,13 +2494,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C89" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D89" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2508,13 +2508,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C90" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D90" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2522,13 +2522,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C91" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D91" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2536,13 +2536,13 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C92" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D92" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2550,13 +2550,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C93" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D93" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2564,13 +2564,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C94" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D94" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2578,13 +2578,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D95" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2592,13 +2592,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C96" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D96" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2606,13 +2606,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C97" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D97" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2620,13 +2620,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C98" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D98" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2634,13 +2634,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C99" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D99" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2648,13 +2648,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C100" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D100" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2662,13 +2662,13 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C101" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D101" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2676,13 +2676,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C102" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D102" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2690,13 +2690,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D103" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2704,13 +2704,13 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C104" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D104" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2718,13 +2718,13 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C105" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D105" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2732,13 +2732,13 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C106" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D106" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2746,13 +2746,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C107" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D107" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2760,13 +2760,13 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C108" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D108" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2774,13 +2774,13 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C109" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D109" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2788,13 +2788,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C110" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D110" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2802,13 +2802,13 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C111" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D111" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2816,13 +2816,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C112" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D112" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2830,13 +2830,13 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C113" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D113" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2844,13 +2844,13 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C114" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D114" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2858,13 +2858,13 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C115" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D115" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2872,13 +2872,13 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C116" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D116" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2886,13 +2886,13 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C117" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D117" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,13 +2900,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C118" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D118" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2914,13 +2914,13 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C119" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D119" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2928,13 +2928,13 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C120" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D120" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2942,13 +2942,13 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C121" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D121" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2956,13 +2956,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C122" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D122" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2970,13 +2970,13 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C123" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D123" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2984,13 +2984,13 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C124" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D124" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2998,13 +2998,13 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C125" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D125" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3012,13 +3012,13 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C126" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D126" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3026,13 +3026,13 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C127" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D127" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3040,13 +3040,13 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C128" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D128" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3054,10 +3054,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C129" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D129" t="s">
         <v>4</v>
@@ -3080,11 +3080,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.28515625" bestFit="1" customWidth="1"/>
@@ -3093,7 +3093,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3107,7 +3107,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3118,7 +3118,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3126,10 +3126,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3137,10 +3137,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3148,10 +3148,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3159,10 +3159,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -3170,10 +3170,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3181,10 +3181,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -3192,10 +3192,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3203,10 +3203,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -3214,10 +3214,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -3225,10 +3225,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -3236,10 +3236,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" t="s">
         <v>258</v>
-      </c>
-      <c r="B14" t="s">
-        <v>260</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -3247,10 +3247,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B15" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -3258,10 +3258,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B16" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -3269,10 +3269,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C17">
         <v>3</v>
@@ -3280,10 +3280,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C18">
         <v>4</v>
@@ -3291,10 +3291,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C19">
         <v>5</v>
@@ -3302,10 +3302,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C20">
         <v>6</v>
@@ -3326,6 +3326,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -3566,42 +3587,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B964A4-BD34-45DC-A0C1-F7E06137407B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3624,9 +3613,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86B964A4-BD34-45DC-A0C1-F7E06137407B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changing Dataschema in P1 and P2 to ISCED-2011 Standard
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF108BD9-EC6D-4B81-9906-F93C9804C1FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBE91B7-173A-4B3C-BD29-E3D3E1F04F4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="286">
   <si>
     <t>index</t>
   </si>
@@ -763,24 +763,6 @@
     <t>female</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>primary school completed</t>
-  </si>
-  <si>
-    <t>technical/professional school completed</t>
-  </si>
-  <si>
-    <t>secondary school</t>
-  </si>
-  <si>
-    <t>longer education (incl. university)</t>
-  </si>
-  <si>
-    <t>not specified</t>
-  </si>
-  <si>
     <t>never</t>
   </si>
   <si>
@@ -875,6 +857,36 @@
   </si>
   <si>
     <t>Body Mass Index at baseline [kg/m²]</t>
+  </si>
+  <si>
+    <t>Early Childhood Education</t>
+  </si>
+  <si>
+    <t>Primary Education</t>
+  </si>
+  <si>
+    <t>Lower Secondary Education</t>
+  </si>
+  <si>
+    <t>Upper Secondary Education</t>
+  </si>
+  <si>
+    <t>Post-secondary non-tertiary education</t>
+  </si>
+  <si>
+    <t>Short-Cycle Tertiary Education</t>
+  </si>
+  <si>
+    <t>Bachelor's or equivalent level</t>
+  </si>
+  <si>
+    <t>Master's or equivalent level</t>
+  </si>
+  <si>
+    <t>Doctoral or equivalent level</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -929,9 +941,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -947,7 +959,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1245,11 +1257,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625"/>
     <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
@@ -1276,10 +1288,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -1307,7 +1319,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1335,7 +1347,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1363,7 +1375,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1741,7 +1753,7 @@
         <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -1755,7 +1767,7 @@
         <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -1797,7 +1809,7 @@
         <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -1825,7 +1837,7 @@
         <v>76</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -1937,7 +1949,7 @@
         <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -2077,7 +2089,7 @@
         <v>110</v>
       </c>
       <c r="C59" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -2091,7 +2103,7 @@
         <v>111</v>
       </c>
       <c r="C60" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -2217,7 +2229,7 @@
         <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
@@ -2245,7 +2257,7 @@
         <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
@@ -2413,7 +2425,7 @@
         <v>154</v>
       </c>
       <c r="C83" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D83" t="s">
         <v>11</v>
@@ -2511,7 +2523,7 @@
         <v>167</v>
       </c>
       <c r="C90" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D90" t="s">
         <v>11</v>
@@ -2903,7 +2915,7 @@
         <v>222</v>
       </c>
       <c r="C118" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D118" t="s">
         <v>11</v>
@@ -2945,7 +2957,7 @@
         <v>227</v>
       </c>
       <c r="C121" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D121" t="s">
         <v>11</v>
@@ -3043,7 +3055,7 @@
         <v>240</v>
       </c>
       <c r="C128" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D128" t="s">
         <v>11</v>
@@ -3054,10 +3066,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C129" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D129" t="s">
         <v>4</v>
@@ -3078,13 +3090,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.28515625" bestFit="1" customWidth="1"/>
@@ -3129,7 +3141,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>276</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3140,7 +3152,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>277</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3151,7 +3163,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>278</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3162,7 +3174,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>247</v>
+        <v>279</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -3173,7 +3185,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3184,7 +3196,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>249</v>
+        <v>281</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -3192,126 +3204,170 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>250</v>
+        <v>282</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>251</v>
+        <v>283</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>253</v>
+        <v>285</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>256</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>256</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>256</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B19" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B20" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21" t="s">
+        <v>253</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>250</v>
+      </c>
+      <c r="B22" t="s">
+        <v>255</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23" t="s">
+        <v>254</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>250</v>
+      </c>
+      <c r="B24" t="s">
+        <v>270</v>
+      </c>
+      <c r="C24">
         <v>6</v>
       </c>
     </row>
-    <row r="64" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{85760D7C-312A-4647-B300-A227B229A527}">
@@ -3326,15 +3382,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -3344,6 +3391,15 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3588,14 +3644,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -3608,6 +3656,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added reference to ISCED 2011 in the variables description of the Dataschema
</commit_message>
<xml_diff>
--- a/rmonize/data_schema/Dataschema_P1.xlsx
+++ b/rmonize/data_schema/Dataschema_P1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBE91B7-173A-4B3C-BD29-E3D3E1F04F4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5138F8-0C10-4C96-A966-A88556A7E43C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>EDU_LEVEL</t>
   </si>
   <si>
-    <t>Education</t>
-  </si>
-  <si>
     <t>TOT_PA_QX</t>
   </si>
   <si>
@@ -887,6 +884,9 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Highest level of education [ISCED 2011]</t>
   </si>
 </sst>
 </file>
@@ -1257,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,10 +1288,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" t="s">
         <v>248</v>
-      </c>
-      <c r="C2" t="s">
-        <v>249</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -1319,10 +1319,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1333,7 +1333,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>285</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -1344,13 +1344,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1358,10 +1358,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -1372,13 +1372,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1386,13 +1386,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1400,13 +1400,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1414,13 +1414,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1428,13 +1428,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1442,13 +1442,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1456,13 +1456,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1470,13 +1470,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1484,13 +1484,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1498,13 +1498,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1512,13 +1512,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1526,13 +1526,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1540,13 +1540,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1554,13 +1554,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="C21" t="s">
-        <v>40</v>
-      </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1568,13 +1568,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
-        <v>42</v>
-      </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1582,13 +1582,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
         <v>43</v>
       </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1596,13 +1596,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
         <v>45</v>
       </c>
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1610,13 +1610,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
         <v>47</v>
       </c>
-      <c r="C25" t="s">
-        <v>48</v>
-      </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1624,13 +1624,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1638,13 +1638,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1652,13 +1652,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
         <v>53</v>
       </c>
-      <c r="C28" t="s">
-        <v>54</v>
-      </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1666,13 +1666,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
         <v>55</v>
       </c>
-      <c r="C29" t="s">
-        <v>56</v>
-      </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1680,13 +1680,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
         <v>57</v>
       </c>
-      <c r="C30" t="s">
-        <v>58</v>
-      </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1694,13 +1694,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
         <v>59</v>
       </c>
-      <c r="C31" t="s">
-        <v>60</v>
-      </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1708,13 +1708,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
         <v>61</v>
       </c>
-      <c r="C32" t="s">
-        <v>62</v>
-      </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1722,13 +1722,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
         <v>63</v>
       </c>
-      <c r="C33" t="s">
-        <v>64</v>
-      </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1736,13 +1736,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" t="s">
         <v>65</v>
       </c>
-      <c r="C34" t="s">
-        <v>66</v>
-      </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1750,13 +1750,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1764,13 +1764,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1778,13 +1778,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
         <v>69</v>
       </c>
-      <c r="C37" t="s">
-        <v>70</v>
-      </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1792,13 +1792,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" t="s">
         <v>71</v>
       </c>
-      <c r="C38" t="s">
-        <v>72</v>
-      </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1806,13 +1806,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1820,13 +1820,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" t="s">
         <v>74</v>
       </c>
-      <c r="C40" t="s">
-        <v>75</v>
-      </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1834,13 +1834,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1848,13 +1848,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" t="s">
         <v>77</v>
       </c>
-      <c r="C42" t="s">
-        <v>78</v>
-      </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1862,13 +1862,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
         <v>79</v>
       </c>
-      <c r="C43" t="s">
-        <v>80</v>
-      </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1876,13 +1876,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
         <v>81</v>
       </c>
-      <c r="C44" t="s">
-        <v>82</v>
-      </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,13 +1890,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" t="s">
         <v>83</v>
       </c>
-      <c r="C45" t="s">
-        <v>84</v>
-      </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1904,13 +1904,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" t="s">
         <v>85</v>
       </c>
-      <c r="C46" t="s">
-        <v>86</v>
-      </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,13 +1918,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" t="s">
         <v>87</v>
       </c>
-      <c r="C47" t="s">
-        <v>88</v>
-      </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1932,13 +1932,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" t="s">
         <v>89</v>
       </c>
-      <c r="C48" t="s">
-        <v>90</v>
-      </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1946,13 +1946,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1960,13 +1960,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50" t="s">
         <v>92</v>
       </c>
-      <c r="C50" t="s">
-        <v>93</v>
-      </c>
       <c r="D50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1974,13 +1974,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" t="s">
         <v>94</v>
       </c>
-      <c r="C51" t="s">
-        <v>95</v>
-      </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1988,13 +1988,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" t="s">
         <v>96</v>
       </c>
-      <c r="C52" t="s">
-        <v>97</v>
-      </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2002,13 +2002,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
         <v>98</v>
       </c>
-      <c r="C53" t="s">
-        <v>99</v>
-      </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2016,13 +2016,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" t="s">
         <v>100</v>
       </c>
-      <c r="C54" t="s">
-        <v>101</v>
-      </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2030,13 +2030,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" t="s">
         <v>102</v>
       </c>
-      <c r="C55" t="s">
-        <v>103</v>
-      </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -2044,13 +2044,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" t="s">
         <v>104</v>
       </c>
-      <c r="C56" t="s">
-        <v>105</v>
-      </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2058,13 +2058,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" t="s">
         <v>106</v>
       </c>
-      <c r="C57" t="s">
-        <v>107</v>
-      </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2072,13 +2072,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" t="s">
         <v>108</v>
       </c>
-      <c r="C58" t="s">
-        <v>109</v>
-      </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2086,13 +2086,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C59" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2100,13 +2100,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C60" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2114,13 +2114,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" t="s">
         <v>112</v>
       </c>
-      <c r="C61" t="s">
-        <v>113</v>
-      </c>
       <c r="D61" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2128,13 +2128,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" t="s">
         <v>114</v>
       </c>
-      <c r="C62" t="s">
-        <v>115</v>
-      </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2142,13 +2142,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>115</v>
+      </c>
+      <c r="C63" t="s">
         <v>116</v>
       </c>
-      <c r="C63" t="s">
-        <v>117</v>
-      </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2156,13 +2156,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>117</v>
+      </c>
+      <c r="C64" t="s">
         <v>118</v>
       </c>
-      <c r="C64" t="s">
-        <v>119</v>
-      </c>
       <c r="D64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2170,13 +2170,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" t="s">
         <v>120</v>
       </c>
-      <c r="C65" t="s">
-        <v>121</v>
-      </c>
       <c r="D65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2184,13 +2184,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" t="s">
         <v>122</v>
       </c>
-      <c r="C66" t="s">
-        <v>123</v>
-      </c>
       <c r="D66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2198,13 +2198,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>123</v>
+      </c>
+      <c r="C67" t="s">
         <v>124</v>
       </c>
-      <c r="C67" t="s">
-        <v>125</v>
-      </c>
       <c r="D67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,13 +2212,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" t="s">
         <v>126</v>
       </c>
-      <c r="C68" t="s">
-        <v>127</v>
-      </c>
       <c r="D68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2226,13 +2226,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C69" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2240,13 +2240,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" t="s">
         <v>129</v>
       </c>
-      <c r="C70" t="s">
-        <v>130</v>
-      </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2254,13 +2254,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C71" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2268,13 +2268,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
+        <v>131</v>
+      </c>
+      <c r="C72" t="s">
         <v>132</v>
       </c>
-      <c r="C72" t="s">
-        <v>133</v>
-      </c>
       <c r="D72" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2282,13 +2282,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
+        <v>133</v>
+      </c>
+      <c r="C73" t="s">
         <v>134</v>
       </c>
-      <c r="C73" t="s">
-        <v>135</v>
-      </c>
       <c r="D73" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2296,13 +2296,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" t="s">
         <v>136</v>
       </c>
-      <c r="C74" t="s">
-        <v>137</v>
-      </c>
       <c r="D74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2310,13 +2310,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" t="s">
         <v>138</v>
       </c>
-      <c r="C75" t="s">
-        <v>139</v>
-      </c>
       <c r="D75" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2324,13 +2324,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
+        <v>139</v>
+      </c>
+      <c r="C76" t="s">
         <v>140</v>
       </c>
-      <c r="C76" t="s">
-        <v>141</v>
-      </c>
       <c r="D76" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2338,13 +2338,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" t="s">
         <v>142</v>
       </c>
-      <c r="C77" t="s">
-        <v>143</v>
-      </c>
       <c r="D77" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2352,13 +2352,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>143</v>
+      </c>
+      <c r="C78" t="s">
         <v>144</v>
       </c>
-      <c r="C78" t="s">
-        <v>145</v>
-      </c>
       <c r="D78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2366,13 +2366,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>145</v>
+      </c>
+      <c r="C79" t="s">
         <v>146</v>
       </c>
-      <c r="C79" t="s">
-        <v>147</v>
-      </c>
       <c r="D79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2380,13 +2380,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>147</v>
+      </c>
+      <c r="C80" t="s">
         <v>148</v>
       </c>
-      <c r="C80" t="s">
-        <v>149</v>
-      </c>
       <c r="D80" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,13 +2394,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
+        <v>149</v>
+      </c>
+      <c r="C81" t="s">
         <v>150</v>
       </c>
-      <c r="C81" t="s">
-        <v>151</v>
-      </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2408,13 +2408,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
+        <v>151</v>
+      </c>
+      <c r="C82" t="s">
         <v>152</v>
       </c>
-      <c r="C82" t="s">
-        <v>153</v>
-      </c>
       <c r="D82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2422,13 +2422,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C83" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2436,13 +2436,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" t="s">
         <v>155</v>
       </c>
-      <c r="C84" t="s">
-        <v>156</v>
-      </c>
       <c r="D84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2450,13 +2450,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
+        <v>156</v>
+      </c>
+      <c r="C85" t="s">
         <v>157</v>
       </c>
-      <c r="C85" t="s">
-        <v>158</v>
-      </c>
       <c r="D85" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2464,13 +2464,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
+        <v>158</v>
+      </c>
+      <c r="C86" t="s">
         <v>159</v>
       </c>
-      <c r="C86" t="s">
-        <v>160</v>
-      </c>
       <c r="D86" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2478,13 +2478,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
+        <v>160</v>
+      </c>
+      <c r="C87" t="s">
         <v>161</v>
       </c>
-      <c r="C87" t="s">
-        <v>162</v>
-      </c>
       <c r="D87" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2492,13 +2492,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
+        <v>162</v>
+      </c>
+      <c r="C88" t="s">
         <v>163</v>
       </c>
-      <c r="C88" t="s">
-        <v>164</v>
-      </c>
       <c r="D88" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2506,13 +2506,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
+        <v>164</v>
+      </c>
+      <c r="C89" t="s">
         <v>165</v>
       </c>
-      <c r="C89" t="s">
-        <v>166</v>
-      </c>
       <c r="D89" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2520,13 +2520,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C90" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2534,13 +2534,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91" t="s">
         <v>168</v>
       </c>
-      <c r="C91" t="s">
-        <v>169</v>
-      </c>
       <c r="D91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2548,13 +2548,13 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
+        <v>169</v>
+      </c>
+      <c r="C92" t="s">
         <v>170</v>
       </c>
-      <c r="C92" t="s">
-        <v>171</v>
-      </c>
       <c r="D92" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2562,13 +2562,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
+        <v>171</v>
+      </c>
+      <c r="C93" t="s">
         <v>172</v>
       </c>
-      <c r="C93" t="s">
-        <v>173</v>
-      </c>
       <c r="D93" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2576,13 +2576,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
+        <v>173</v>
+      </c>
+      <c r="C94" t="s">
         <v>174</v>
       </c>
-      <c r="C94" t="s">
-        <v>175</v>
-      </c>
       <c r="D94" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2590,13 +2590,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
+        <v>175</v>
+      </c>
+      <c r="C95" t="s">
         <v>176</v>
       </c>
-      <c r="C95" t="s">
-        <v>177</v>
-      </c>
       <c r="D95" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2604,13 +2604,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
+        <v>177</v>
+      </c>
+      <c r="C96" t="s">
         <v>178</v>
       </c>
-      <c r="C96" t="s">
-        <v>179</v>
-      </c>
       <c r="D96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2618,13 +2618,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" t="s">
         <v>180</v>
       </c>
-      <c r="C97" t="s">
-        <v>181</v>
-      </c>
       <c r="D97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2632,13 +2632,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
+        <v>181</v>
+      </c>
+      <c r="C98" t="s">
         <v>182</v>
       </c>
-      <c r="C98" t="s">
-        <v>183</v>
-      </c>
       <c r="D98" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2646,13 +2646,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
+        <v>183</v>
+      </c>
+      <c r="C99" t="s">
         <v>184</v>
       </c>
-      <c r="C99" t="s">
-        <v>185</v>
-      </c>
       <c r="D99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2660,13 +2660,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
+        <v>185</v>
+      </c>
+      <c r="C100" t="s">
         <v>186</v>
       </c>
-      <c r="C100" t="s">
-        <v>187</v>
-      </c>
       <c r="D100" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2674,13 +2674,13 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
+        <v>187</v>
+      </c>
+      <c r="C101" t="s">
         <v>188</v>
       </c>
-      <c r="C101" t="s">
-        <v>189</v>
-      </c>
       <c r="D101" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2688,13 +2688,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
+        <v>189</v>
+      </c>
+      <c r="C102" t="s">
         <v>190</v>
       </c>
-      <c r="C102" t="s">
-        <v>191</v>
-      </c>
       <c r="D102" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2702,13 +2702,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" t="s">
         <v>192</v>
       </c>
-      <c r="C103" t="s">
-        <v>193</v>
-      </c>
       <c r="D103" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2716,13 +2716,13 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
+        <v>193</v>
+      </c>
+      <c r="C104" t="s">
         <v>194</v>
       </c>
-      <c r="C104" t="s">
-        <v>195</v>
-      </c>
       <c r="D104" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2730,13 +2730,13 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
+        <v>195</v>
+      </c>
+      <c r="C105" t="s">
         <v>196</v>
       </c>
-      <c r="C105" t="s">
-        <v>197</v>
-      </c>
       <c r="D105" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -2744,13 +2744,13 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
+        <v>197</v>
+      </c>
+      <c r="C106" t="s">
         <v>198</v>
       </c>
-      <c r="C106" t="s">
-        <v>199</v>
-      </c>
       <c r="D106" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2758,13 +2758,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
+        <v>199</v>
+      </c>
+      <c r="C107" t="s">
         <v>200</v>
       </c>
-      <c r="C107" t="s">
-        <v>201</v>
-      </c>
       <c r="D107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -2772,13 +2772,13 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
+        <v>201</v>
+      </c>
+      <c r="C108" t="s">
         <v>202</v>
       </c>
-      <c r="C108" t="s">
-        <v>203</v>
-      </c>
       <c r="D108" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -2786,13 +2786,13 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" t="s">
         <v>204</v>
       </c>
-      <c r="C109" t="s">
-        <v>205</v>
-      </c>
       <c r="D109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -2800,13 +2800,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
+        <v>205</v>
+      </c>
+      <c r="C110" t="s">
         <v>206</v>
       </c>
-      <c r="C110" t="s">
-        <v>207</v>
-      </c>
       <c r="D110" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2814,13 +2814,13 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
+        <v>207</v>
+      </c>
+      <c r="C111" t="s">
         <v>208</v>
       </c>
-      <c r="C111" t="s">
-        <v>209</v>
-      </c>
       <c r="D111" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -2828,13 +2828,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
+        <v>209</v>
+      </c>
+      <c r="C112" t="s">
         <v>210</v>
       </c>
-      <c r="C112" t="s">
-        <v>211</v>
-      </c>
       <c r="D112" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -2842,13 +2842,13 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
+        <v>211</v>
+      </c>
+      <c r="C113" t="s">
         <v>212</v>
       </c>
-      <c r="C113" t="s">
-        <v>213</v>
-      </c>
       <c r="D113" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -2856,13 +2856,13 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
+        <v>213</v>
+      </c>
+      <c r="C114" t="s">
         <v>214</v>
       </c>
-      <c r="C114" t="s">
-        <v>215</v>
-      </c>
       <c r="D114" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -2870,13 +2870,13 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
+        <v>215</v>
+      </c>
+      <c r="C115" t="s">
         <v>216</v>
       </c>
-      <c r="C115" t="s">
-        <v>217</v>
-      </c>
       <c r="D115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2884,13 +2884,13 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
+        <v>217</v>
+      </c>
+      <c r="C116" t="s">
         <v>218</v>
       </c>
-      <c r="C116" t="s">
-        <v>219</v>
-      </c>
       <c r="D116" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2898,13 +2898,13 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
+        <v>219</v>
+      </c>
+      <c r="C117" t="s">
         <v>220</v>
       </c>
-      <c r="C117" t="s">
-        <v>221</v>
-      </c>
       <c r="D117" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2912,13 +2912,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C118" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D118" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2926,13 +2926,13 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
+        <v>222</v>
+      </c>
+      <c r="C119" t="s">
         <v>223</v>
       </c>
-      <c r="C119" t="s">
-        <v>224</v>
-      </c>
       <c r="D119" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2940,13 +2940,13 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
+        <v>224</v>
+      </c>
+      <c r="C120" t="s">
         <v>225</v>
       </c>
-      <c r="C120" t="s">
-        <v>226</v>
-      </c>
       <c r="D120" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2954,13 +2954,13 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C121" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D121" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2968,13 +2968,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
+        <v>227</v>
+      </c>
+      <c r="C122" t="s">
         <v>228</v>
       </c>
-      <c r="C122" t="s">
-        <v>229</v>
-      </c>
       <c r="D122" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2982,13 +2982,13 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
+        <v>229</v>
+      </c>
+      <c r="C123" t="s">
         <v>230</v>
       </c>
-      <c r="C123" t="s">
-        <v>231</v>
-      </c>
       <c r="D123" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2996,13 +2996,13 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
+        <v>231</v>
+      </c>
+      <c r="C124" t="s">
         <v>232</v>
       </c>
-      <c r="C124" t="s">
-        <v>233</v>
-      </c>
       <c r="D124" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -3010,13 +3010,13 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
+        <v>233</v>
+      </c>
+      <c r="C125" t="s">
         <v>234</v>
       </c>
-      <c r="C125" t="s">
-        <v>235</v>
-      </c>
       <c r="D125" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -3024,13 +3024,13 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>235</v>
+      </c>
+      <c r="C126" t="s">
         <v>236</v>
       </c>
-      <c r="C126" t="s">
-        <v>237</v>
-      </c>
       <c r="D126" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3038,13 +3038,13 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
+        <v>237</v>
+      </c>
+      <c r="C127" t="s">
         <v>238</v>
       </c>
-      <c r="C127" t="s">
-        <v>239</v>
-      </c>
       <c r="D127" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3052,13 +3052,13 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C128" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D128" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -3066,10 +3066,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
+        <v>249</v>
+      </c>
+      <c r="C129" t="s">
         <v>250</v>
-      </c>
-      <c r="C129" t="s">
-        <v>251</v>
       </c>
       <c r="D129" t="s">
         <v>4</v>
@@ -3092,7 +3092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:C13"/>
     </sheetView>
   </sheetViews>
@@ -3105,7 +3105,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -3119,7 +3119,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3130,7 +3130,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3141,7 +3141,7 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3152,7 +3152,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3163,7 +3163,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3174,7 +3174,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -3185,7 +3185,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -3196,7 +3196,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -3207,7 +3207,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -3218,7 +3218,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -3229,7 +3229,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -3240,7 +3240,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C13">
         <v>9</v>
@@ -3248,10 +3248,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3259,10 +3259,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -3270,10 +3270,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -3281,10 +3281,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -3292,10 +3292,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -3303,10 +3303,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -3314,10 +3314,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -3325,10 +3325,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -3336,10 +3336,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -3347,10 +3347,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -3358,10 +3358,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C24">
         <v>6</v>
@@ -3382,6 +3382,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -3391,15 +3400,6 @@
     <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3644,6 +3644,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EB6D834-F5F1-4875-9BFF-E74D4F6F598A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -3656,14 +3664,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBBE8B2F-371B-4499-AB2D-BE5C88E1FE7D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>